<commit_message>
added time stamp for 29.08.
</commit_message>
<xml_diff>
--- a/documentation/Protocol_Timesheet_Todo.xlsx
+++ b/documentation/Protocol_Timesheet_Todo.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Time Sheet" sheetId="1" state="visible" r:id="rId2"/>
@@ -39,6 +39,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Time Sheet'!$7:$7</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Time Sheet'!$7:$7</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Time Sheet'!$7:$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Time Sheet'!$7:$7</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">'Project Plan'!$B$3:$D$3</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="ColumnTitle1" vbProcedure="false">TimeSheet[[#Headers],[Date(s)]]</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Protocol!$B$3:$C$3</definedName>
@@ -60,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="89">
   <si>
     <t xml:space="preserve">Time Sheet</t>
   </si>
@@ -169,6 +170,12 @@
     <t xml:space="preserve">OpenCV + Tensorflow tutorial on cat/dog problem</t>
   </si>
   <si>
+    <t xml:space="preserve">28.08.2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">29.08.2018</t>
+  </si>
+  <si>
     <t xml:space="preserve">TODO</t>
   </si>
   <si>
@@ -262,9 +269,6 @@
     <t xml:space="preserve">Problems with Ubuntu on the PC → unmet dependencies</t>
   </si>
   <si>
-    <t xml:space="preserve">24.08.2019</t>
-  </si>
-  <si>
     <t xml:space="preserve">Ubuntu problem could not be solved → contacted uni IT services</t>
   </si>
   <si>
@@ -272,6 +276,24 @@
   </si>
   <si>
     <t xml:space="preserve">moved stuff to the NTU github</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pedro solved the Linux Problem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Team meeting with Sabrina and Quentin → This week will be focused on familiarizing with Quentins Framework</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wrote message to Georgina → One-Shot learning is too much work; the available code for zero-shot learning is not usable for us</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Searching for new papers on One-Shot Learning</t>
+  </si>
+  <si>
+    <t xml:space="preserve">An external camera would be useful instead of the sawyers head-camera → using the Kinect camera in the lab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wrote email to Chelsea Finn (cbfinn@eecs.berkeley.edu) → asking about the source code to its paper “One-Shot Imitation from Observing Humans via Domain-Adaptive Meta-Learning”</t>
   </si>
   <si>
     <t xml:space="preserve">Ordered</t>
@@ -889,9 +911,9 @@
     <tabColor rgb="FF273645"/>
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="B1:I17"/>
+  <dimension ref="B1:I19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H18" activeCellId="0" sqref="H18"/>
     </sheetView>
   </sheetViews>
@@ -969,7 +991,7 @@
       </c>
       <c r="C6" s="10" t="n">
         <f aca="false">SUBTOTAL(109,TimeSheet[Hours Worked])</f>
-        <v>67</v>
+        <v>74.5</v>
       </c>
       <c r="D6" s="10" t="n">
         <f aca="false">IFERROR(IF(C6&lt;=WorkweekHours,C6,WorkweekHours),"")</f>
@@ -977,7 +999,7 @@
       </c>
       <c r="E6" s="10" t="n">
         <f aca="false">IFERROR(C6-D6, "")</f>
-        <v>32</v>
+        <v>39.5</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="40" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1245,9 +1267,42 @@
         <v>34</v>
       </c>
     </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="16" t="n">
+        <v>0.385416666666667</v>
+      </c>
+      <c r="D18" s="16" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E18" s="16" t="n">
+        <v>0.541666666666667</v>
+      </c>
+      <c r="F18" s="16" t="n">
+        <v>0.739583333333333</v>
+      </c>
+      <c r="G18" s="15" t="n">
+        <f aca="false">IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Lunch End]]+TimeSheet[[#This Row],[Lunch Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" s="16" t="n">
+        <v>0.40625</v>
+      </c>
+      <c r="G19" s="15" t="n">
+        <f aca="false">IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Lunch End]]+TimeSheet[[#This Row],[Lunch Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="25">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C1:AMJ1 A2:A9 F2:AMJ2 D3:AMJ4 F5:AMJ6 H7:AMJ7 B8:AMJ9 G10:G17" type="none">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C1:AMJ1 A2:A9 F2:AMJ2 D3:AMJ4 F5:AMJ6 H7:AMJ7 B8:AMJ9 G10:G19" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -1387,45 +1442,45 @@
   <sheetData>
     <row r="1" customFormat="false" ht="36.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B1" s="18" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C1" s="18"/>
       <c r="D1" s="18"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="19" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D4" s="21"/>
     </row>
     <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="0" t="s">
         <v>42</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1522,7 +1577,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="32" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C1" s="24"/>
       <c r="D1" s="24"/>
@@ -1533,13 +1588,13 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C2" s="25" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D2" s="26" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="E2" s="26" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1573,10 +1628,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:H32"/>
+  <dimension ref="B1:H40"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C38" activeCellId="0" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1591,7 +1646,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="32" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C1" s="24"/>
       <c r="D1" s="24"/>
@@ -1602,7 +1657,7 @@
     </row>
     <row r="3" s="22" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="11" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C3" s="11" t="s">
         <v>17</v>
@@ -1610,24 +1665,24 @@
     </row>
     <row r="4" s="22" customFormat="true" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="22" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" s="22" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="6" s="22" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="22" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" s="22" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C7" s="22" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1636,32 +1691,32 @@
         <v>26</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C10" s="23" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C11" s="23" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C12" s="23" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="23" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C14" s="23" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1670,7 +1725,7 @@
         <v>28</v>
       </c>
       <c r="C16" s="23" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1689,22 +1744,22 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C20" s="23" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C21" s="23" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C22" s="23" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C23" s="23" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1713,46 +1768,79 @@
         <v>31</v>
       </c>
       <c r="C25" s="23" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C26" s="23" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C27" s="23" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="22" t="s">
-        <v>66</v>
+        <v>33</v>
       </c>
       <c r="C29" s="23" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C30" s="23" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C31" s="23" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B33" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C33" s="23" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C34" s="23" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C35" s="23" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C36" s="23" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C37" s="23" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B38" s="0"/>
+      <c r="C38" s="0"/>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B39" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="C39" s="23" t="s">
+        <v>76</v>
+      </c>
+    </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1895,6 +1983,7 @@
     <hyperlink ref="C16" r:id="rId4" display="Installed all requirements for zero-shot imitation learning as described here: https://github.com/pathak22/zeroshot-imitation"/>
     <hyperlink ref="C21" r:id="rId5" display="Tutorial on “Image Difference with OpenCV and Python” (https://www.pyimagesearch.com/2017/06/19/image-difference-with-opencv-and-python/)"/>
     <hyperlink ref="C22" r:id="rId6" display="Tutorial on “OpenCV shape detection” (https://www.pyimagesearch.com/2016/02/08/opencv-shape-detection/)"/>
+    <hyperlink ref="C39" r:id="rId7" display="cbfinn@eecs.berkeley.edu"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -1904,7 +1993,7 @@
     <oddFooter/>
   </headerFooter>
   <tableParts>
-    <tablePart r:id="rId7"/>
+    <tablePart r:id="rId8"/>
   </tableParts>
 </worksheet>
 </file>
@@ -1936,7 +2025,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="32" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="2" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="C1" s="24"/>
       <c r="D1" s="24"/>
@@ -1949,31 +2038,31 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="11" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="G3" s="33" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="H3" s="34" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="I3" s="34" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="J3" s="34" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2174,7 +2263,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="32" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="2" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="C1" s="24"/>
       <c r="D1" s="24"/>
@@ -2186,28 +2275,28 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="11" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="F3" s="33" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="G3" s="34" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="H3" s="34" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="I3" s="48" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2269,7 +2358,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="32" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="2" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="C1" s="24"/>
     </row>
@@ -2278,10 +2367,10 @@
     </row>
     <row r="3" s="22" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="11" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
added timestep for 31.08.
</commit_message>
<xml_diff>
--- a/documentation/Protocol_Timesheet_Todo.xlsx
+++ b/documentation/Protocol_Timesheet_Todo.xlsx
@@ -5,13 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Time Sheet" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Todo-List" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Project Plan" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="Protocol" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Protocol" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Todo-List" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Project Plan" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="Ordered" sheetId="5" state="visible" r:id="rId6"/>
     <sheet name="To Order" sheetId="6" state="visible" r:id="rId7"/>
     <sheet name="To Discuss" sheetId="7" state="visible" r:id="rId8"/>
@@ -41,9 +41,10 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Time Sheet'!$7:$7</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Time Sheet'!$7:$7</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Time Sheet'!$7:$7</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">'Project Plan'!$B$3:$D$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="ColumnTitle1" vbProcedure="false">TimeSheet[[#Headers],[Date(s)]]</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Protocol!$B$3:$C$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Time Sheet'!$7:$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="ColumnTitle1" vbProcedure="false">TimeSheet[[#Headers],[Date(s)]]</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">Protocol!$B$3:$C$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">'Project Plan'!$B$3:$D$3</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="ColumnTitle1" vbProcedure="false">TimeSheet[[#Headers],[Date(s)]]</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">Ordered!$B$3:$C$3</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="ColumnTitle1" vbProcedure="false">TimeSheet[[#Headers],[Date(s)]]</definedName>
@@ -62,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="100">
   <si>
     <t xml:space="preserve">Time Sheet</t>
   </si>
@@ -174,9 +175,129 @@
     <t xml:space="preserve">28.08.2018</t>
   </si>
   <si>
+    <t xml:space="preserve">Research on new papers about one-shot learning</t>
+  </si>
+  <si>
     <t xml:space="preserve">29.08.2018</t>
   </si>
   <si>
+    <t xml:space="preserve">30.08.2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Installing requirements for one-shot learning from human observation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">31.08.2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Protocol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13.08.2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Account created</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14.08.2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Setting up Unix</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tutorial on ROS http://wiki.ros.org/ROS/Tutorials until 7.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Finished draft of literature review</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ros Tutorial until 10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Installed all requirements for zero-shot imitation learning as described here: https://github.com/pathak22/zeroshot-imitation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“make” fails → cublas_v2.h: No such file or directory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tried to install CUDA Toolkit from https://developer.nvidia.com/cuda-downloads?target_os=Linux&amp;target_arch=x86_64&amp;target_distro=Ubuntu&amp;target_version=1710&amp;target_type=runfilelocal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Disk space is too small → “Need 6836686400 bytes”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Installed OpenCV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tutorial on “Image Difference with OpenCV and Python” (https://www.pyimagesearch.com/2017/06/19/image-difference-with-opencv-and-python/)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tutorial on “OpenCV shape detection” (https://www.pyimagesearch.com/2016/02/08/opencv-shape-detection/)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Playing around with the Shape detection algorithm: own shapes and changing the parameters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OpenCV course on “color detection” → testing on sample image of sawyer robot → robot arm can be detected</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OpenCV course on “object tracking” → testing on sample video of sawyer robot → robot arm can be detected</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Problems with Ubuntu on the PC → unmet dependencies</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ubuntu problem could not be solved → contacted uni IT services</t>
+  </si>
+  <si>
+    <t xml:space="preserve">changed to different pc and istalled everything there</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moved stuff to the NTU github</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pedro solved the Linux Problem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Team meeting with Sabrina and Quentin → This week will be focused on familiarizing with Quentins Framework</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wrote message to Georgina → One-Shot learning is too much work; the available code for zero-shot learning is not usable for us</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Searching for new papers on One-Shot Learning</t>
+  </si>
+  <si>
+    <t xml:space="preserve">An external camera would be useful instead of the sawyers head-camera → using the Kinect camera in the lab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wrote email to Chelsea Finn (cbfinn@eecs.berkeley.edu) → asking about the source code to its paper “One-Shot Imitation from Observing Humans via Domain-Adaptive Meta-Learning”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Got response from Chelsea Finn → The code can be found at their github https://github.com/tianheyu927/mil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Installed all requirements for the one-shot learning algorithm on the virtual machine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">it is required to download MuJoCo, which is just available for free if you are student</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MujoCo is a physics engine to simulate the environment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Also OpenAI Gym is needed, which is a toolkit for developing and comparing reinforcement learning algorithms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The training data is &gt;25GB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">made tutorial on object recognition using the VGG dataset https://machinelearningmastery.com/use-pre-trained-vgg-model-classify-objects-photographs/</t>
+  </si>
+  <si>
     <t xml:space="preserve">TODO</t>
   </si>
   <si>
@@ -186,9 +307,6 @@
     <t xml:space="preserve">Done?</t>
   </si>
   <si>
-    <t xml:space="preserve">Date</t>
-  </si>
-  <si>
     <t xml:space="preserve">ROS Tutorial</t>
   </si>
   <si>
@@ -211,114 +329,6 @@
   </si>
   <si>
     <t xml:space="preserve">Steps</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Protocol</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13.08.2018</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Account created</t>
-  </si>
-  <si>
-    <t xml:space="preserve">14.08.2018</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Setting up Unix</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tutorial on ROS http://wiki.ros.org/ROS/Tutorials until 7.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Finished draft of literature review</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ros Tutorial until 10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Installed all requirements for zero-shot imitation learning as described here: https://github.com/pathak22/zeroshot-imitation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">“make” fails → cublas_v2.h: No such file or directory</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tried to install CUDA Toolkit from https://developer.nvidia.com/cuda-downloads?target_os=Linux&amp;target_arch=x86_64&amp;target_distro=Ubuntu&amp;target_version=1710&amp;target_type=runfilelocal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Disk space is too small → “Need 6836686400 bytes”</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Installed OpenCV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tutorial on “Image Difference with OpenCV and Python” (https://www.pyimagesearch.com/2017/06/19/image-difference-with-opencv-and-python/)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tutorial on “OpenCV shape detection” (https://www.pyimagesearch.com/2016/02/08/opencv-shape-detection/)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Playing around with the Shape detection algorithm: own shapes and changing the parameters</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OpenCV course on “color detection” → testing on sample image of sawyer robot → robot arm can be detected</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OpenCV course on “object tracking” → testing on sample video of sawyer robot → robot arm can be detected</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Problems with Ubuntu on the PC → unmet dependencies</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ubuntu problem could not be solved → contacted uni IT services</t>
-  </si>
-  <si>
-    <t xml:space="preserve">changed to different pc and istalled everything there</t>
-  </si>
-  <si>
-    <t xml:space="preserve">moved stuff to the NTU github</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pedro solved the Linux Problem</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Team meeting with Sabrina and Quentin → This week will be focused on familiarizing with Quentins Framework</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wrote message to Georgina → One-Shot learning is too much work; the available code for zero-shot learning is not usable for us</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Searching for new papers on One-Shot Learning</t>
-  </si>
-  <si>
-    <t xml:space="preserve">An external camera would be useful instead of the sawyers head-camera → using the Kinect camera in the lab</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wrote email to Chelsea Finn (cbfinn@eecs.berkeley.edu) → asking about the source code to its paper “One-Shot Imitation from Observing Humans via Domain-Adaptive Meta-Learning”</t>
-  </si>
-  <si>
-    <t xml:space="preserve">30.08.2018</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Got response from Chelsea Finn → The code can be found at their github https://github.com/tianheyu927/mil</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Installed all requirements for the one-shot learning algorithm on the virtual machine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">it is required to download MuJoCo, which is just available for free if you are student</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MujoCo is a physics engine to simulate the environment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Also OpenAI Gym is needed, which is a toolkit for developing and comparing reinforcement learning algorithms</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The training data is &gt;25GB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">made tutorial on object recognition using the VGG dataset https://machinelearningmastery.com/use-pre-trained-vgg-model-classify-objects-photographs/</t>
   </si>
   <si>
     <t xml:space="preserve">Ordered</t>
@@ -563,6 +573,26 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -583,31 +613,11 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="171" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -936,10 +946,10 @@
     <tabColor rgb="FF273645"/>
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="B1:I19"/>
+  <dimension ref="B1:I21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H18" activeCellId="0" sqref="H18"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H21" activeCellId="0" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1016,7 +1026,7 @@
       </c>
       <c r="C6" s="10" t="n">
         <f aca="false">SUBTOTAL(109,TimeSheet[Hours Worked])</f>
-        <v>74.5</v>
+        <v>88.0000000000001</v>
       </c>
       <c r="D6" s="10" t="n">
         <f aca="false">IFERROR(IF(C6&lt;=WorkweekHours,C6,WorkweekHours),"")</f>
@@ -1024,7 +1034,7 @@
       </c>
       <c r="E6" s="10" t="n">
         <f aca="false">IFERROR(C6-D6, "")</f>
-        <v>39.5</v>
+        <v>53.0000000000001</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="40" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1121,7 +1131,7 @@
       </c>
       <c r="G10" s="15" t="n">
         <f aca="false">IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Lunch End]]+TimeSheet[[#This Row],[Lunch Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
-        <v>6.00000000000001</v>
+        <v>6.00000000000003</v>
       </c>
       <c r="H10" s="0" t="s">
         <v>21</v>
@@ -1145,7 +1155,7 @@
       </c>
       <c r="G11" s="15" t="n">
         <f aca="false">IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Lunch End]]+TimeSheet[[#This Row],[Lunch Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
-        <v>7.25000000000001</v>
+        <v>7.25000000000002</v>
       </c>
       <c r="H11" s="0" t="s">
         <v>23</v>
@@ -1169,7 +1179,7 @@
       </c>
       <c r="G12" s="15" t="n">
         <f aca="false">IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Lunch End]]+TimeSheet[[#This Row],[Lunch Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
-        <v>6.25</v>
+        <v>6.25000000000001</v>
       </c>
       <c r="H12" s="0" t="s">
         <v>25</v>
@@ -1241,7 +1251,7 @@
       </c>
       <c r="G15" s="15" t="n">
         <f aca="false">IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Lunch End]]+TimeSheet[[#This Row],[Lunch Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
-        <v>7.50000000000001</v>
+        <v>7.50000000000002</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1262,7 +1272,7 @@
       </c>
       <c r="G16" s="15" t="n">
         <f aca="false">IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Lunch End]]+TimeSheet[[#This Row],[Lunch Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
-        <v>7.5</v>
+        <v>7.50000000000003</v>
       </c>
       <c r="H16" s="0" t="s">
         <v>32</v>
@@ -1286,7 +1296,7 @@
       </c>
       <c r="G17" s="15" t="n">
         <f aca="false">IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Lunch End]]+TimeSheet[[#This Row],[Lunch Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
-        <v>6.74999999999999</v>
+        <v>6.75</v>
       </c>
       <c r="H17" s="0" t="s">
         <v>34</v>
@@ -1310,24 +1320,68 @@
       </c>
       <c r="G18" s="15" t="n">
         <f aca="false">IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Lunch End]]+TimeSheet[[#This Row],[Lunch Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
-        <v>7.5</v>
+        <v>7.49999999999998</v>
+      </c>
+      <c r="H18" s="0" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C19" s="16" t="n">
         <v>0.40625</v>
       </c>
+      <c r="D19" s="16" t="n">
+        <v>0.510416666666667</v>
+      </c>
+      <c r="E19" s="16" t="n">
+        <v>0.552083333333333</v>
+      </c>
+      <c r="F19" s="16" t="n">
+        <v>0.729166666666667</v>
+      </c>
       <c r="G19" s="15" t="n">
         <f aca="false">IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Lunch End]]+TimeSheet[[#This Row],[Lunch Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
-        <v>0</v>
+        <v>6.75</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" s="16" t="n">
+        <v>0.40625</v>
+      </c>
+      <c r="D20" s="16" t="n">
+        <v>0.510416666666667</v>
+      </c>
+      <c r="E20" s="16" t="n">
+        <v>0.552083333333333</v>
+      </c>
+      <c r="F20" s="16" t="n">
+        <v>0.729166666666667</v>
+      </c>
+      <c r="G20" s="15" t="n">
+        <f aca="false">IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Lunch End]]+TimeSheet[[#This Row],[Lunch Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
+        <v>6.75</v>
+      </c>
+      <c r="H20" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="16" t="n">
+        <v>0.385416666666667</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="25">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C1:AMJ1 A2:A9 F2:AMJ2 D3:AMJ4 F5:AMJ6 H7:AMJ7 B8:AMJ9 G10:G19" type="none">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C1:AMJ1 A2:A9 F2:AMJ2 D3:AMJ4 F5:AMJ6 H7:AMJ7 B8:AMJ9 G10:G20" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -1449,409 +1503,205 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:D7"/>
+  <dimension ref="B1:H48"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="2.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="52.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="17" width="21.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="8.83"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="36.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B1" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="C3" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="D3" s="20" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="D4" s="21"/>
-    </row>
-    <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-  </sheetData>
-  <conditionalFormatting sqref="C2:C14 C16 C18 C29:C1048576 C27 C20:C24">
-    <cfRule type="containsText" priority="2" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="no" dxfId="0"/>
-    <cfRule type="containsText" priority="3" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="yes" dxfId="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C19">
-    <cfRule type="containsText" priority="4" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="no" dxfId="2"/>
-    <cfRule type="containsText" priority="5" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="yes" dxfId="3"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C28">
-    <cfRule type="containsText" priority="6" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="no" dxfId="4"/>
-    <cfRule type="containsText" priority="7" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="yes" dxfId="5"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C17">
-    <cfRule type="containsText" priority="8" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="no" dxfId="6"/>
-    <cfRule type="containsText" priority="9" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="yes" dxfId="7"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C26">
-    <cfRule type="containsText" priority="10" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="no" dxfId="8"/>
-    <cfRule type="containsText" priority="11" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="yes" dxfId="9"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C25">
-    <cfRule type="containsText" priority="12" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="no" dxfId="10"/>
-    <cfRule type="containsText" priority="13" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="yes" dxfId="11"/>
-  </conditionalFormatting>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-  <tableParts>
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="B1:H3"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="22" width="2.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="22" width="20.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="23" width="13.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="23" width="10.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="22" width="28.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="22" width="19.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="22" width="8.83"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="32" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C2" s="25" t="s">
-        <v>46</v>
-      </c>
-      <c r="D2" s="26" t="s">
-        <v>47</v>
-      </c>
-      <c r="E2" s="26" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-  </sheetData>
-  <dataValidations count="2">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C1:H1" type="none">
-      <formula1>0</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="between" prompt="Title of this worksheet is in this cell.  Enter Employee and Manager details in cells below" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B1" type="none">
-      <formula1>0</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-  </dataValidations>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="B1:H48"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D47" activeCellId="0" sqref="D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="22" width="2.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="22" width="13.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="23" width="127"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="23" width="12.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="22" width="47.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="22" width="8.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="17" width="2.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="17" width="13.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="18" width="127"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="18" width="12.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="17" width="47.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="17" width="8.83"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="32" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
+        <v>41</v>
+      </c>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
     </row>
-    <row r="3" s="22" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="11" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C3" s="11" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" s="22" customFormat="true" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="22" t="s">
-        <v>50</v>
-      </c>
-      <c r="C4" s="27" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="5" s="22" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="6" s="22" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="22" t="s">
-        <v>52</v>
-      </c>
-      <c r="C6" s="22" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="7" s="22" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C7" s="22" t="s">
-        <v>54</v>
+    <row r="4" s="17" customFormat="true" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" s="17" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="6" s="17" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C7" s="17" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="22" t="s">
+      <c r="B9" s="17" t="s">
         <v>26</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C10" s="23" t="s">
-        <v>56</v>
+      <c r="C10" s="18" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C11" s="23" t="s">
-        <v>57</v>
+      <c r="C11" s="18" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C12" s="23" t="s">
-        <v>58</v>
+      <c r="C12" s="18" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C13" s="23" t="s">
-        <v>59</v>
+      <c r="C13" s="18" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C14" s="23" t="s">
-        <v>60</v>
+      <c r="C14" s="18" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="22" t="s">
+      <c r="B16" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="C16" s="23" t="s">
-        <v>57</v>
+      <c r="C16" s="18" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C17" s="28" t="s">
+      <c r="C17" s="21" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="22" t="s">
+      <c r="B19" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="C19" s="28" t="s">
+      <c r="C19" s="21" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C20" s="23" t="s">
-        <v>61</v>
+      <c r="C20" s="18" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C21" s="23" t="s">
-        <v>62</v>
+      <c r="C21" s="18" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C22" s="23" t="s">
-        <v>63</v>
+      <c r="C22" s="18" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C23" s="23" t="s">
-        <v>64</v>
+      <c r="C23" s="18" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="22" t="s">
+      <c r="B25" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="C25" s="23" t="s">
-        <v>65</v>
+      <c r="C25" s="18" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C26" s="23" t="s">
-        <v>66</v>
+      <c r="C26" s="18" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C27" s="23" t="s">
-        <v>67</v>
+      <c r="C27" s="18" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="22" t="s">
+      <c r="B29" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="C29" s="23" t="s">
-        <v>68</v>
+      <c r="C29" s="18" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C30" s="23" t="s">
-        <v>69</v>
+      <c r="C30" s="18" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C31" s="23" t="s">
-        <v>70</v>
+      <c r="C31" s="18" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="22" t="s">
+      <c r="B33" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="C33" s="23" t="s">
-        <v>71</v>
+      <c r="C33" s="18" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C34" s="23" t="s">
-        <v>72</v>
+      <c r="C34" s="18" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C35" s="23" t="s">
-        <v>73</v>
+      <c r="C35" s="18" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C36" s="23" t="s">
-        <v>74</v>
+      <c r="C36" s="18" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C37" s="23" t="s">
-        <v>75</v>
+      <c r="C37" s="18" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1859,50 +1709,50 @@
       <c r="C38" s="0"/>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="C39" s="23" t="s">
-        <v>76</v>
+      <c r="B39" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="C39" s="18" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B41" s="22" t="s">
-        <v>77</v>
-      </c>
-      <c r="C41" s="23" t="s">
-        <v>78</v>
+      <c r="B41" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="C41" s="18" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C42" s="23" t="s">
-        <v>79</v>
+      <c r="C42" s="18" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C43" s="23" t="s">
-        <v>80</v>
+      <c r="C43" s="18" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C44" s="23" t="s">
-        <v>81</v>
+      <c r="C44" s="18" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C45" s="23" t="s">
-        <v>82</v>
+      <c r="C45" s="18" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C46" s="23" t="s">
-        <v>83</v>
+      <c r="C46" s="18" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C47" s="23" t="s">
-        <v>84</v>
+      <c r="C47" s="18" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2040,8 +1890,8 @@
     <hyperlink ref="C21" r:id="rId5" display="Tutorial on “Image Difference with OpenCV and Python” (https://www.pyimagesearch.com/2017/06/19/image-difference-with-opencv-and-python/)"/>
     <hyperlink ref="C22" r:id="rId6" display="Tutorial on “OpenCV shape detection” (https://www.pyimagesearch.com/2016/02/08/opencv-shape-detection/)"/>
     <hyperlink ref="C39" r:id="rId7" display="Wrote email to Chelsea Finn (cbfinn@eecs.berkeley.edu) → asking about the source code to its paper “One-Shot Imitation from Observing Humans via Domain-Adaptive Meta-Learning”"/>
-    <hyperlink ref="C41" r:id="rId8" display="https://github.com/tianheyu927/mil"/>
-    <hyperlink ref="C47" r:id="rId9" display="https://machinelearningmastery.com/use-pre-trained-vgg-model-classify-objects-photographs/"/>
+    <hyperlink ref="C41" r:id="rId8" display="Got response from Chelsea Finn → The code can be found at their github https://github.com/tianheyu927/mil"/>
+    <hyperlink ref="C47" r:id="rId9" display="made tutorial on object recognition using the VGG dataset https://machinelearningmastery.com/use-pre-trained-vgg-model-classify-objects-photographs/"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -2053,6 +1903,210 @@
   <tableParts>
     <tablePart r:id="rId10"/>
   </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="B1:D7"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="2.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="52.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="22" width="21.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="8.83"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="36.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B1" s="23" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="C3" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="D3" s="25" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="D4" s="26"/>
+    </row>
+    <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <conditionalFormatting sqref="C2:C14 C16 C18 C29:C1048576 C27 C20:C24">
+    <cfRule type="containsText" priority="2" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="no" dxfId="0"/>
+    <cfRule type="containsText" priority="3" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="yes" dxfId="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C19">
+    <cfRule type="containsText" priority="4" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="no" dxfId="2"/>
+    <cfRule type="containsText" priority="5" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="yes" dxfId="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C28">
+    <cfRule type="containsText" priority="6" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="no" dxfId="4"/>
+    <cfRule type="containsText" priority="7" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="yes" dxfId="5"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C17">
+    <cfRule type="containsText" priority="8" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="no" dxfId="6"/>
+    <cfRule type="containsText" priority="9" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="yes" dxfId="7"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C26">
+    <cfRule type="containsText" priority="10" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="no" dxfId="8"/>
+    <cfRule type="containsText" priority="11" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="yes" dxfId="9"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C25">
+    <cfRule type="containsText" priority="12" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="no" dxfId="10"/>
+    <cfRule type="containsText" priority="13" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="yes" dxfId="11"/>
+  </conditionalFormatting>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+  <tableParts>
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="B1:H3"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="17" width="2.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="17" width="20.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="18" width="13.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="18" width="10.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="17" width="28.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="17" width="19.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="17" width="8.83"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="32" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C2" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="D2" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="E2" s="28" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C1:H1" type="none">
+      <formula1>0</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="between" prompt="Title of this worksheet is in this cell.  Enter Employee and Manager details in cells below" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B1" type="none">
+      <formula1>0</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -2069,26 +2123,26 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="22" width="2.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="22" width="13.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="23" width="21.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="23" width="28.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="22" width="24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="22" width="27.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="17" width="2.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="17" width="13.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="18" width="21.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="18" width="28.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="17" width="24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="17" width="27.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="29" width="8.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="30" width="13.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="30" width="10.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="22" width="8.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="17" width="8.83"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="32" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
+        <v>88</v>
+      </c>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
       <c r="G1" s="31"/>
       <c r="H1" s="32"/>
       <c r="I1" s="32"/>
@@ -2096,64 +2150,64 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="11" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="G3" s="33" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="H3" s="34" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="I3" s="34" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="J3" s="34" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
       <c r="G4" s="35"/>
       <c r="H4" s="36"/>
       <c r="I4" s="37"/>
       <c r="J4" s="37"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C5" s="22"/>
-      <c r="D5" s="22"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
       <c r="H5" s="38"/>
       <c r="J5" s="30"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C6" s="22"/>
-      <c r="D6" s="22"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
       <c r="H6" s="38"/>
       <c r="J6" s="30"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C7" s="22"/>
-      <c r="D7" s="22"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
       <c r="H7" s="38"/>
       <c r="J7" s="30"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C8" s="22"/>
-      <c r="D8" s="22"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
       <c r="H8" s="38"/>
       <c r="J8" s="30"/>
     </row>
@@ -2171,36 +2225,36 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="5"/>
-      <c r="C10" s="22"/>
-      <c r="D10" s="22"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
       <c r="H10" s="38"/>
       <c r="J10" s="30"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="5"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="22"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
       <c r="H11" s="38"/>
       <c r="J11" s="30"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="5"/>
-      <c r="C12" s="22"/>
-      <c r="D12" s="22"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
       <c r="H12" s="38"/>
       <c r="J12" s="30"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="5"/>
-      <c r="C13" s="22"/>
-      <c r="D13" s="22"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
       <c r="H13" s="38"/>
       <c r="J13" s="30"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="5"/>
-      <c r="C14" s="22"/>
-      <c r="D14" s="22"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
       <c r="H14" s="38"/>
       <c r="J14" s="30"/>
     </row>
@@ -2249,7 +2303,7 @@
       <c r="J18" s="30"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C19" s="22"/>
+      <c r="C19" s="17"/>
       <c r="F19" s="29"/>
       <c r="I19" s="42"/>
       <c r="J19" s="30"/>
@@ -2307,54 +2361,54 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="22" width="2.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="22" width="26.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="23" width="28.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="23" width="28.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="22" width="24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="22" width="8.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="17" width="2.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="17" width="26.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="18" width="28.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="18" width="28.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="17" width="24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="17" width="8.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="29" width="13.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="30" width="10.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="30" width="12.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="22" width="8.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="17" width="8.83"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="32" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
+        <v>97</v>
+      </c>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
       <c r="G1" s="31"/>
       <c r="H1" s="32"/>
       <c r="I1" s="32"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="11" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="F3" s="33" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="G3" s="34" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="H3" s="34" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="I3" s="48" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2402,33 +2456,33 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="22" width="2.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="22" width="31.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="23" width="65.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="23" width="28.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="22" width="24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="22" width="8.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="17" width="2.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="17" width="31.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="18" width="65.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="18" width="28.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="17" width="24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="17" width="8.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="29" width="13.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="30" width="10.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="30" width="12.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="22" width="8.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="17" width="8.83"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="32" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="C1" s="24"/>
-    </row>
-    <row r="2" s="22" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C2" s="23"/>
-    </row>
-    <row r="3" s="22" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>98</v>
+      </c>
+      <c r="C1" s="19"/>
+    </row>
+    <row r="2" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C2" s="18"/>
+    </row>
+    <row r="3" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="11" t="s">
-        <v>38</v>
+        <v>78</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
added time stamp for 3.09.
</commit_message>
<xml_diff>
--- a/documentation/Protocol_Timesheet_Todo.xlsx
+++ b/documentation/Protocol_Timesheet_Todo.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Time Sheet" sheetId="1" state="visible" r:id="rId2"/>
@@ -42,6 +42,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Time Sheet'!$7:$7</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Time Sheet'!$7:$7</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Time Sheet'!$7:$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Time Sheet'!$7:$7</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="ColumnTitle1" vbProcedure="false">TimeSheet[[#Headers],[Date(s)]]</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">Protocol!$B$3:$C$3</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">'Project Plan'!$B$3:$D$3</definedName>
@@ -63,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="104">
   <si>
     <t xml:space="preserve">Time Sheet</t>
   </si>
@@ -190,6 +191,12 @@
     <t xml:space="preserve">31.08.2018</t>
   </si>
   <si>
+    <t xml:space="preserve">03.09.2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Installing software for Kinect Camera</t>
+  </si>
+  <si>
     <t xml:space="preserve">Protocol</t>
   </si>
   <si>
@@ -296,6 +303,12 @@
   </si>
   <si>
     <t xml:space="preserve">made tutorial on object recognition using the VGG dataset https://machinelearningmastery.com/use-pre-trained-vgg-model-classify-objects-photographs/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tried to install software for the Kinect camera at the workstation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">There is no USB 3.0 at the PC so the Kinect can not be used → setting everything up on a different computer</t>
   </si>
   <si>
     <t xml:space="preserve">TODO</t>
@@ -946,10 +959,10 @@
     <tabColor rgb="FF273645"/>
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="B1:I21"/>
+  <dimension ref="B1:I22"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H21" activeCellId="0" sqref="H21"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H23" activeCellId="0" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1026,7 +1039,7 @@
       </c>
       <c r="C6" s="10" t="n">
         <f aca="false">SUBTOTAL(109,TimeSheet[Hours Worked])</f>
-        <v>88.0000000000001</v>
+        <v>103.25</v>
       </c>
       <c r="D6" s="10" t="n">
         <f aca="false">IFERROR(IF(C6&lt;=WorkweekHours,C6,WorkweekHours),"")</f>
@@ -1034,7 +1047,7 @@
       </c>
       <c r="E6" s="10" t="n">
         <f aca="false">IFERROR(C6-D6, "")</f>
-        <v>53.0000000000001</v>
+        <v>68.2500000000001</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="40" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1378,10 +1391,47 @@
       <c r="C21" s="16" t="n">
         <v>0.385416666666667</v>
       </c>
+      <c r="D21" s="16" t="n">
+        <v>0.510416666666667</v>
+      </c>
+      <c r="E21" s="16" t="n">
+        <v>0.552083333333333</v>
+      </c>
+      <c r="F21" s="16" t="n">
+        <v>0.708333333333333</v>
+      </c>
+      <c r="G21" s="15" t="n">
+        <f aca="false">IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Lunch End]]+TimeSheet[[#This Row],[Lunch Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
+        <v>6.74999999999999</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B22" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22" s="16" t="n">
+        <v>0.385416666666667</v>
+      </c>
+      <c r="D22" s="16" t="n">
+        <v>0.510416666666667</v>
+      </c>
+      <c r="E22" s="16" t="n">
+        <v>0.552083333333333</v>
+      </c>
+      <c r="F22" s="16" t="n">
+        <v>0.78125</v>
+      </c>
+      <c r="G22" s="15" t="n">
+        <f aca="false">IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Lunch End]]+TimeSheet[[#This Row],[Lunch Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
+        <v>8.5</v>
+      </c>
+      <c r="H22" s="0" t="s">
+        <v>42</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="25">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C1:AMJ1 A2:A9 F2:AMJ2 D3:AMJ4 F5:AMJ6 H7:AMJ7 B8:AMJ9 G10:G20" type="none">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C1:AMJ1 A2:A9 F2:AMJ2 D3:AMJ4 F5:AMJ6 H7:AMJ7 B8:AMJ9 G10:G22" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -1503,10 +1553,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:H48"/>
+  <dimension ref="B1:H51"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D47" activeCellId="0" sqref="D47"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C51" activeCellId="0" sqref="C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1521,7 +1571,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="32" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C1" s="19"/>
       <c r="D1" s="19"/>
@@ -1532,7 +1582,7 @@
     </row>
     <row r="3" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="11" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C3" s="11" t="s">
         <v>17</v>
@@ -1540,24 +1590,24 @@
     </row>
     <row r="4" s="17" customFormat="true" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="17" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" s="17" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="6" s="17" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="17" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C7" s="17" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1566,32 +1616,32 @@
         <v>26</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C10" s="18" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C11" s="18" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C12" s="18" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="18" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C14" s="18" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1600,7 +1650,7 @@
         <v>28</v>
       </c>
       <c r="C16" s="18" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1619,22 +1669,22 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C20" s="18" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C21" s="18" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C22" s="18" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C23" s="18" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1643,17 +1693,17 @@
         <v>31</v>
       </c>
       <c r="C25" s="18" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C26" s="18" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C27" s="18" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1662,17 +1712,17 @@
         <v>33</v>
       </c>
       <c r="C29" s="18" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C30" s="18" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C31" s="18" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1681,27 +1731,27 @@
         <v>35</v>
       </c>
       <c r="C33" s="18" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C34" s="18" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C35" s="18" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C36" s="18" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C37" s="18" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1713,7 +1763,7 @@
         <v>37</v>
       </c>
       <c r="C39" s="18" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1722,42 +1772,53 @@
         <v>38</v>
       </c>
       <c r="C41" s="18" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C42" s="18" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C43" s="18" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C44" s="18" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C45" s="18" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C46" s="18" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C47" s="18" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B49" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="C49" s="18" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C50" s="18" t="s">
+        <v>80</v>
+      </c>
+    </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1929,45 +1990,45 @@
   <sheetData>
     <row r="1" customFormat="false" ht="36.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B1" s="23" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="C1" s="23"/>
       <c r="D1" s="23"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="24" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="C3" s="24" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="D3" s="25" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="D4" s="26"/>
     </row>
     <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2064,7 +2125,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="32" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="2" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="C1" s="19"/>
       <c r="D1" s="19"/>
@@ -2075,13 +2136,13 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C2" s="27" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="D2" s="28" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="E2" s="28" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2137,7 +2198,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="32" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="2" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="C1" s="19"/>
       <c r="D1" s="19"/>
@@ -2150,31 +2211,31 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="11" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="G3" s="33" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="H3" s="34" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="I3" s="34" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="J3" s="34" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2375,7 +2436,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="32" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="2" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="C1" s="19"/>
       <c r="D1" s="19"/>
@@ -2387,28 +2448,28 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="11" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="F3" s="33" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="G3" s="34" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="H3" s="34" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="I3" s="48" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2470,7 +2531,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="32" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="2" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="C1" s="19"/>
     </row>
@@ -2479,10 +2540,10 @@
     </row>
     <row r="3" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="11" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
added time stamp for 5.09.2018
</commit_message>
<xml_diff>
--- a/documentation/Protocol_Timesheet_Todo.xlsx
+++ b/documentation/Protocol_Timesheet_Todo.xlsx
@@ -44,6 +44,8 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Time Sheet'!$7:$7</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Time Sheet'!$7:$7</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Time Sheet'!$7:$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Time Sheet'!$7:$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Time Sheet'!$7:$7</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="ColumnTitle1" vbProcedure="false">TimeSheet[[#Headers],[Date(s)]]</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">Protocol!$B$3:$C$3</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">'Project Plan'!$B$3:$D$3</definedName>
@@ -65,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="111">
   <si>
     <t xml:space="preserve">Time Sheet</t>
   </si>
@@ -204,6 +206,9 @@
     <t xml:space="preserve">Installing software for Kinect Camera, Documentation in the Wiki, Testing the camera</t>
   </si>
   <si>
+    <t xml:space="preserve">05.09.2018</t>
+  </si>
+  <si>
     <t xml:space="preserve">Protocol</t>
   </si>
   <si>
@@ -325,6 +330,9 @@
   </si>
   <si>
     <t xml:space="preserve">Testing → Color, IR and depth pictures</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contacted Chelsea Finn to ask for a sample demonstration file for the Sawyer robot</t>
   </si>
   <si>
     <t xml:space="preserve">TODO</t>
@@ -975,10 +983,10 @@
     <tabColor rgb="FF273645"/>
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="B1:I23"/>
+  <dimension ref="B1:I24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F23" activeCellId="0" sqref="F23"/>
+      <selection pane="topLeft" activeCell="H27" activeCellId="0" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1055,7 +1063,7 @@
       </c>
       <c r="C6" s="10" t="n">
         <f aca="false">SUBTOTAL(109,TimeSheet[Hours Worked])</f>
-        <v>103.25</v>
+        <v>118.75</v>
       </c>
       <c r="D6" s="10" t="n">
         <f aca="false">IFERROR(IF(C6&lt;=WorkweekHours,C6,WorkweekHours),"")</f>
@@ -1063,7 +1071,7 @@
       </c>
       <c r="E6" s="10" t="n">
         <f aca="false">IFERROR(C6-D6, "")</f>
-        <v>68.2500000000001</v>
+        <v>83.7500000000001</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="40" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1458,17 +1466,41 @@
       <c r="E23" s="16" t="n">
         <v>0.552083333333333</v>
       </c>
+      <c r="F23" s="16" t="n">
+        <v>0.770833333333333</v>
+      </c>
       <c r="G23" s="15" t="n">
         <f aca="false">IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Lunch End]]+TimeSheet[[#This Row],[Lunch Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
-        <v>0</v>
+        <v>8.00000000000003</v>
       </c>
       <c r="H23" s="0" t="s">
         <v>44</v>
       </c>
     </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B24" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="C24" s="16" t="n">
+        <v>0.385416666666667</v>
+      </c>
+      <c r="D24" s="16" t="n">
+        <v>0.541666666666667</v>
+      </c>
+      <c r="E24" s="16" t="n">
+        <v>0.572916666666667</v>
+      </c>
+      <c r="F24" s="16" t="n">
+        <v>0.729166666666667</v>
+      </c>
+      <c r="G24" s="15" t="n">
+        <f aca="false">IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Lunch End]]+TimeSheet[[#This Row],[Lunch Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
+        <v>7.49999999999999</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="25">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C1:AMJ1 A2:A9 F2:AMJ2 D3:AMJ4 F5:AMJ6 H7:AMJ7 B8:AMJ9 G10:G23" type="none">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C1:AMJ1 A2:A9 F2:AMJ2 D3:AMJ4 F5:AMJ6 H7:AMJ7 B8:AMJ9 G10:G24" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -1590,10 +1622,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:H55"/>
+  <dimension ref="B1:H57"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C55" activeCellId="0" sqref="C55"/>
+      <selection pane="topLeft" activeCell="B57" activeCellId="0" sqref="B57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1608,7 +1640,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="32" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C1" s="19"/>
       <c r="D1" s="19"/>
@@ -1619,7 +1651,7 @@
     </row>
     <row r="3" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="11" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C3" s="11" t="s">
         <v>17</v>
@@ -1627,24 +1659,24 @@
     </row>
     <row r="4" s="17" customFormat="true" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="17" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" s="17" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="6" s="17" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="17" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C7" s="17" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1653,32 +1685,32 @@
         <v>26</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C10" s="18" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C11" s="18" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C12" s="18" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="18" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C14" s="18" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1687,7 +1719,7 @@
         <v>28</v>
       </c>
       <c r="C16" s="18" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1706,22 +1738,22 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C20" s="18" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C21" s="18" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C22" s="18" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C23" s="18" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1730,17 +1762,17 @@
         <v>31</v>
       </c>
       <c r="C25" s="18" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C26" s="18" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C27" s="18" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1749,17 +1781,17 @@
         <v>33</v>
       </c>
       <c r="C29" s="18" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C30" s="18" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C31" s="18" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1768,27 +1800,27 @@
         <v>35</v>
       </c>
       <c r="C33" s="18" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C34" s="18" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C35" s="18" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C36" s="18" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C37" s="18" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1800,7 +1832,7 @@
         <v>37</v>
       </c>
       <c r="C39" s="18" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1809,37 +1841,37 @@
         <v>38</v>
       </c>
       <c r="C41" s="18" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C42" s="18" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C43" s="18" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C44" s="18" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C45" s="18" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C46" s="18" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C47" s="18" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1848,12 +1880,12 @@
         <v>41</v>
       </c>
       <c r="C49" s="18" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C50" s="18" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1862,21 +1894,28 @@
         <v>43</v>
       </c>
       <c r="C52" s="18" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C53" s="18" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C54" s="18" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B56" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="C56" s="18" t="s">
+        <v>87</v>
+      </c>
+    </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2042,45 +2081,45 @@
   <sheetData>
     <row r="1" customFormat="false" ht="36.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B1" s="23" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C1" s="23"/>
       <c r="D1" s="23"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="24" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C3" s="24" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="D3" s="25" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D4" s="26"/>
     </row>
     <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="C6" s="0" t="s">
         <v>92</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2177,7 +2216,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="32" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C1" s="19"/>
       <c r="D1" s="19"/>
@@ -2188,13 +2227,13 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C2" s="27" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D2" s="28" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="E2" s="28" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2250,7 +2289,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="32" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C1" s="19"/>
       <c r="D1" s="19"/>
@@ -2263,31 +2302,31 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="11" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="G3" s="33" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="H3" s="34" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="I3" s="34" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="J3" s="34" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2488,7 +2527,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="32" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="2" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C1" s="19"/>
       <c r="D1" s="19"/>
@@ -2500,28 +2539,28 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="11" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="F3" s="33" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="G3" s="34" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="H3" s="34" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="I3" s="48" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2583,7 +2622,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="32" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="2" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C1" s="19"/>
     </row>
@@ -2592,10 +2631,10 @@
     </row>
     <row r="3" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="11" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
added protocol for 13.09.
</commit_message>
<xml_diff>
--- a/documentation/Protocol_Timesheet_Todo.xlsx
+++ b/documentation/Protocol_Timesheet_Todo.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Time Sheet" sheetId="1" state="visible" r:id="rId2"/>
@@ -48,6 +48,8 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Time Sheet'!$7:$7</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Time Sheet'!$7:$7</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Time Sheet'!$7:$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Time Sheet'!$7:$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Time Sheet'!$7:$7</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="ColumnTitle1" vbProcedure="false">TimeSheet[[#Headers],[Date(s)]]</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">Protocol!$B$3:$C$3</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">'Project Plan'!$B$3:$D$3</definedName>
@@ -69,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="129">
   <si>
     <t xml:space="preserve">Time Sheet</t>
   </si>
@@ -214,6 +216,15 @@
     <t xml:space="preserve">10.09.2018</t>
   </si>
   <si>
+    <t xml:space="preserve">11.09.2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12.09.20118</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13.09.2018</t>
+  </si>
+  <si>
     <t xml:space="preserve">Protocol</t>
   </si>
   <si>
@@ -341,6 +352,52 @@
   </si>
   <si>
     <t xml:space="preserve">Installed ROS Melodic on the second computer where the Kinect is running</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Replaced the main computer that controls the robot to a different one with USB 3.0 and Ubuntu 18.04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12.09.2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tutorial on “Training YOLOv3 to detect custom objects” (https://medium.com/@manivannan_data/how-to-train-yolov3-to-detect-custom-objects-ccbcafeb13d2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implemented YOLO to detect live objects from the kinect camera</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Started training on custom objects → about 18h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cloned ROLO repository</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  File "./experiments/testing/ROLO_network_test_all.py", line 31
+    from tensorflow.python.ops.rnn_cell
+                                      ^
+SyntaxError: invalid syntax
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">--&gt; change the line "from tensorflow.models.rnn import rnn, rnn_cell" to "from tensorflow.python.ops.rnn_cell import BasicLSTMCell"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Traceback (most recent call last):
+  File "./experiments/testing/ROLO_network_test_all.py", line 27, in &lt;module&gt;
+    import ROLO_utils as utils
+ImportError: No module named ROLO_utils</t>
+  </si>
+  <si>
+    <t xml:space="preserve">--&gt; copy the file utils/ROLO_utils.py to experiments/testing/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tutorial on “Train a Classifier on CIFAR-10” (https://pjreddie.com/darknet/train-cifar/)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">found function on how to move the robot in x y z positions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">table is too low → maybe use a higher table?</t>
   </si>
   <si>
     <t xml:space="preserve">TODO</t>
@@ -906,8 +963,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table25" displayName="Table25" ref="B3:C162" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="B3:C162"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table25" displayName="Table25" ref="B3:C163" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="B3:C163"/>
   <tableColumns count="2">
     <tableColumn id="1" name="Date"/>
     <tableColumn id="2" name="Notes"/>
@@ -991,10 +1048,10 @@
     <tabColor rgb="FF273645"/>
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="B1:I25"/>
+  <dimension ref="B1:I28"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H25" activeCellId="0" sqref="H25"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H28" activeCellId="0" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1071,7 +1128,7 @@
       </c>
       <c r="C6" s="10" t="n">
         <f aca="false">SUBTOTAL(109,TimeSheet[Hours Worked])</f>
-        <v>123.25</v>
+        <v>148</v>
       </c>
       <c r="D6" s="10" t="n">
         <f aca="false">IFERROR(IF(C6&lt;=WorkweekHours,C6,WorkweekHours),"")</f>
@@ -1079,7 +1136,7 @@
       </c>
       <c r="E6" s="10" t="n">
         <f aca="false">IFERROR(C6-D6, "")</f>
-        <v>88.2500000000001</v>
+        <v>113</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="40" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1527,9 +1584,72 @@
         <v>4.5</v>
       </c>
     </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="C26" s="16" t="n">
+        <v>0.385416666666667</v>
+      </c>
+      <c r="D26" s="16" t="n">
+        <v>0.510416666666667</v>
+      </c>
+      <c r="E26" s="16" t="n">
+        <v>0.552083333333333</v>
+      </c>
+      <c r="F26" s="16" t="n">
+        <v>0.8125</v>
+      </c>
+      <c r="G26" s="15" t="n">
+        <f aca="false">IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Lunch End]]+TimeSheet[[#This Row],[Lunch Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
+        <v>9.25</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B27" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="C27" s="16" t="n">
+        <v>0.416666666666667</v>
+      </c>
+      <c r="D27" s="16" t="n">
+        <v>0.510416666666667</v>
+      </c>
+      <c r="E27" s="16" t="n">
+        <v>0.552083333333333</v>
+      </c>
+      <c r="F27" s="16" t="n">
+        <v>0.770833333333333</v>
+      </c>
+      <c r="G27" s="15" t="n">
+        <f aca="false">IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Lunch End]]+TimeSheet[[#This Row],[Lunch Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B28" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="C28" s="16" t="n">
+        <v>0.395833333333333</v>
+      </c>
+      <c r="D28" s="16" t="n">
+        <v>0.510416666666667</v>
+      </c>
+      <c r="E28" s="16" t="n">
+        <v>0.552083333333333</v>
+      </c>
+      <c r="F28" s="16" t="n">
+        <v>0.770833333333333</v>
+      </c>
+      <c r="G28" s="15" t="n">
+        <f aca="false">IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Lunch End]]+TimeSheet[[#This Row],[Lunch Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="25">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C1:AMJ1 A2:A9 F2:AMJ2 D3:AMJ4 F5:AMJ6 H7:AMJ7 B8:AMJ9 G10:G25" type="none">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C1:AMJ1 A2:A9 F2:AMJ2 D3:AMJ4 F5:AMJ6 H7:AMJ7 B8:AMJ9 G10:G28" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -1651,10 +1771,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:H59"/>
+  <dimension ref="B1:H75"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C59" activeCellId="0" sqref="C59"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C75" activeCellId="0" sqref="C75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1669,7 +1789,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="32" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="2" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C1" s="19"/>
       <c r="D1" s="19"/>
@@ -1680,7 +1800,7 @@
     </row>
     <row r="3" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="11" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="C3" s="11" t="s">
         <v>17</v>
@@ -1688,24 +1808,24 @@
     </row>
     <row r="4" s="17" customFormat="true" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="17" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" s="17" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="6" s="17" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="17" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C7" s="17" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1714,32 +1834,32 @@
         <v>26</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C10" s="18" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C11" s="18" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C12" s="18" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="18" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C14" s="18" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1748,7 +1868,7 @@
         <v>28</v>
       </c>
       <c r="C16" s="18" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1767,22 +1887,22 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C20" s="18" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C21" s="18" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C22" s="18" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C23" s="18" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1791,17 +1911,17 @@
         <v>31</v>
       </c>
       <c r="C25" s="18" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C26" s="18" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C27" s="18" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1810,17 +1930,17 @@
         <v>33</v>
       </c>
       <c r="C29" s="18" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C30" s="18" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C31" s="18" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1829,27 +1949,27 @@
         <v>35</v>
       </c>
       <c r="C33" s="18" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C34" s="18" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C35" s="18" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C36" s="18" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C37" s="18" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1861,7 +1981,7 @@
         <v>37</v>
       </c>
       <c r="C39" s="18" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1870,37 +1990,37 @@
         <v>38</v>
       </c>
       <c r="C41" s="18" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C42" s="18" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C43" s="18" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C44" s="18" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C45" s="18" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C46" s="18" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C47" s="18" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1909,12 +2029,12 @@
         <v>41</v>
       </c>
       <c r="C49" s="18" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C50" s="18" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1923,17 +2043,17 @@
         <v>43</v>
       </c>
       <c r="C52" s="18" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C53" s="18" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C54" s="18" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1942,7 +2062,7 @@
         <v>45</v>
       </c>
       <c r="C56" s="18" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1951,25 +2071,82 @@
         <v>46</v>
       </c>
       <c r="C58" s="18" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B60" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="C60" s="18" t="s">
+        <v>93</v>
+      </c>
+    </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B62" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="C62" s="18" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C63" s="18" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C64" s="18" t="s">
+        <v>97</v>
+      </c>
+    </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B66" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="C66" s="18" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="58" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C67" s="20" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C68" s="18" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="47" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C69" s="20" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C70" s="18" t="s">
+        <v>102</v>
+      </c>
+    </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C72" s="18" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C73" s="18" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C74" s="18" t="s">
+        <v>105</v>
+      </c>
+    </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2059,6 +2236,7 @@
     <row r="161" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="162" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="163" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="164" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <dataValidations count="2">
     <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C1:H1" type="none">
@@ -2080,6 +2258,7 @@
     <hyperlink ref="C39" r:id="rId7" display="Wrote email to Chelsea Finn (cbfinn@eecs.berkeley.edu) → asking about the source code to its paper “One-Shot Imitation from Observing Humans via Domain-Adaptive Meta-Learning”"/>
     <hyperlink ref="C41" r:id="rId8" display="Got response from Chelsea Finn → The code can be found at their github https://github.com/tianheyu927/mil"/>
     <hyperlink ref="C47" r:id="rId9" display="made tutorial on object recognition using the VGG dataset https://machinelearningmastery.com/use-pre-trained-vgg-model-classify-objects-photographs/"/>
+    <hyperlink ref="C62" r:id="rId10" display="https://medium.com/@manivannan_data/how-to-train-yolov3-to-detect-custom-objects-ccbcafeb13d2"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -2089,7 +2268,7 @@
     <oddFooter/>
   </headerFooter>
   <tableParts>
-    <tablePart r:id="rId10"/>
+    <tablePart r:id="rId11"/>
   </tableParts>
 </worksheet>
 </file>
@@ -2117,45 +2296,45 @@
   <sheetData>
     <row r="1" customFormat="false" ht="36.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B1" s="23" t="s">
-        <v>90</v>
+        <v>106</v>
       </c>
       <c r="C1" s="23"/>
       <c r="D1" s="23"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="24" t="s">
-        <v>91</v>
+        <v>107</v>
       </c>
       <c r="C3" s="24" t="s">
-        <v>92</v>
+        <v>108</v>
       </c>
       <c r="D3" s="25" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>93</v>
+        <v>109</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>94</v>
+        <v>110</v>
       </c>
       <c r="D4" s="26"/>
     </row>
     <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="s">
-        <v>95</v>
+        <v>111</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>94</v>
+        <v>110</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
-        <v>96</v>
+        <v>112</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>94</v>
+        <v>110</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2252,7 +2431,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="32" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="2" t="s">
-        <v>97</v>
+        <v>113</v>
       </c>
       <c r="C1" s="19"/>
       <c r="D1" s="19"/>
@@ -2263,13 +2442,13 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C2" s="27" t="s">
-        <v>98</v>
+        <v>114</v>
       </c>
       <c r="D2" s="28" t="s">
-        <v>99</v>
+        <v>115</v>
       </c>
       <c r="E2" s="28" t="s">
-        <v>100</v>
+        <v>116</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2325,7 +2504,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="32" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="2" t="s">
-        <v>101</v>
+        <v>117</v>
       </c>
       <c r="C1" s="19"/>
       <c r="D1" s="19"/>
@@ -2338,31 +2517,31 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="11" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>102</v>
+        <v>118</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>103</v>
+        <v>119</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>104</v>
+        <v>120</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>105</v>
+        <v>121</v>
       </c>
       <c r="G3" s="33" t="s">
-        <v>106</v>
+        <v>122</v>
       </c>
       <c r="H3" s="34" t="s">
-        <v>107</v>
+        <v>123</v>
       </c>
       <c r="I3" s="34" t="s">
-        <v>108</v>
+        <v>124</v>
       </c>
       <c r="J3" s="34" t="s">
-        <v>109</v>
+        <v>125</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2563,7 +2742,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="32" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="2" t="s">
-        <v>110</v>
+        <v>126</v>
       </c>
       <c r="C1" s="19"/>
       <c r="D1" s="19"/>
@@ -2575,28 +2754,28 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="11" t="s">
-        <v>102</v>
+        <v>118</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>103</v>
+        <v>119</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>104</v>
+        <v>120</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>105</v>
+        <v>121</v>
       </c>
       <c r="F3" s="33" t="s">
-        <v>106</v>
+        <v>122</v>
       </c>
       <c r="G3" s="34" t="s">
-        <v>107</v>
+        <v>123</v>
       </c>
       <c r="H3" s="34" t="s">
-        <v>108</v>
+        <v>124</v>
       </c>
       <c r="I3" s="48" t="s">
-        <v>109</v>
+        <v>125</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2658,7 +2837,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="32" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="2" t="s">
-        <v>111</v>
+        <v>127</v>
       </c>
       <c r="C1" s="19"/>
     </row>
@@ -2667,10 +2846,10 @@
     </row>
     <row r="3" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="11" t="s">
-        <v>91</v>
+        <v>107</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>112</v>
+        <v>128</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
added timestamp for 14.09
</commit_message>
<xml_diff>
--- a/documentation/Protocol_Timesheet_Todo.xlsx
+++ b/documentation/Protocol_Timesheet_Todo.xlsx
@@ -50,6 +50,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Time Sheet'!$7:$7</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Time Sheet'!$7:$7</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Time Sheet'!$7:$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Time Sheet'!$7:$7</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="ColumnTitle1" vbProcedure="false">TimeSheet[[#Headers],[Date(s)]]</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">Protocol!$B$3:$C$3</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">'Project Plan'!$B$3:$D$3</definedName>
@@ -71,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="134">
   <si>
     <t xml:space="preserve">Time Sheet</t>
   </si>
@@ -223,6 +224,9 @@
   </si>
   <si>
     <t xml:space="preserve">13.09.2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14.09.2018</t>
   </si>
   <si>
     <t xml:space="preserve">Protocol</t>
@@ -398,6 +402,18 @@
   </si>
   <si>
     <t xml:space="preserve">table is too low → maybe use a higher table?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Changed table to the one that is height-adjustable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">taped the region that is reachable by the robot arm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">recorded joint positions of the outer edges of the table</t>
+  </si>
+  <si>
+    <t xml:space="preserve">--&gt; need to convert the coordinates of an object from the Kinect to the robot positions</t>
   </si>
   <si>
     <t xml:space="preserve">TODO</t>
@@ -1048,10 +1064,10 @@
     <tabColor rgb="FF273645"/>
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="B1:I28"/>
+  <dimension ref="B1:I29"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H28" activeCellId="0" sqref="H28"/>
+      <selection pane="topLeft" activeCell="H29" activeCellId="0" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1128,7 +1144,7 @@
       </c>
       <c r="C6" s="10" t="n">
         <f aca="false">SUBTOTAL(109,TimeSheet[Hours Worked])</f>
-        <v>148</v>
+        <v>156.25</v>
       </c>
       <c r="D6" s="10" t="n">
         <f aca="false">IFERROR(IF(C6&lt;=WorkweekHours,C6,WorkweekHours),"")</f>
@@ -1136,7 +1152,7 @@
       </c>
       <c r="E6" s="10" t="n">
         <f aca="false">IFERROR(C6-D6, "")</f>
-        <v>113</v>
+        <v>121.25</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="40" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1647,9 +1663,30 @@
         <v>8</v>
       </c>
     </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B29" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="C29" s="16" t="n">
+        <v>0.385416666666667</v>
+      </c>
+      <c r="D29" s="16" t="n">
+        <v>0.541666666666667</v>
+      </c>
+      <c r="E29" s="16" t="n">
+        <v>0.583333333333333</v>
+      </c>
+      <c r="F29" s="16" t="n">
+        <v>0.770833333333333</v>
+      </c>
+      <c r="G29" s="15" t="n">
+        <f aca="false">IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Lunch End]]+TimeSheet[[#This Row],[Lunch Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
+        <v>8.25</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="25">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C1:AMJ1 A2:A9 F2:AMJ2 D3:AMJ4 F5:AMJ6 H7:AMJ7 B8:AMJ9 G10:G28" type="none">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C1:AMJ1 A2:A9 F2:AMJ2 D3:AMJ4 F5:AMJ6 H7:AMJ7 B8:AMJ9 G10:G29" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -1771,10 +1808,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:H75"/>
+  <dimension ref="B1:H80"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C75" activeCellId="0" sqref="C75"/>
+      <selection pane="topLeft" activeCell="C80" activeCellId="0" sqref="C80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1789,7 +1826,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="32" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C1" s="19"/>
       <c r="D1" s="19"/>
@@ -1800,7 +1837,7 @@
     </row>
     <row r="3" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="11" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C3" s="11" t="s">
         <v>17</v>
@@ -1808,24 +1845,24 @@
     </row>
     <row r="4" s="17" customFormat="true" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="17" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" s="17" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="6" s="17" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="17" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C7" s="17" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1834,32 +1871,32 @@
         <v>26</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C10" s="18" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C11" s="18" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C12" s="18" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="18" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C14" s="18" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1868,7 +1905,7 @@
         <v>28</v>
       </c>
       <c r="C16" s="18" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1887,22 +1924,22 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C20" s="18" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C21" s="18" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C22" s="18" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C23" s="18" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1911,17 +1948,17 @@
         <v>31</v>
       </c>
       <c r="C25" s="18" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C26" s="18" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C27" s="18" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1930,17 +1967,17 @@
         <v>33</v>
       </c>
       <c r="C29" s="18" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C30" s="18" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C31" s="18" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1949,27 +1986,27 @@
         <v>35</v>
       </c>
       <c r="C33" s="18" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C34" s="18" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C35" s="18" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C36" s="18" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C37" s="18" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1981,7 +2018,7 @@
         <v>37</v>
       </c>
       <c r="C39" s="18" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1990,37 +2027,37 @@
         <v>38</v>
       </c>
       <c r="C41" s="18" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C42" s="18" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C43" s="18" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C44" s="18" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C45" s="18" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C46" s="18" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C47" s="18" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2029,12 +2066,12 @@
         <v>41</v>
       </c>
       <c r="C49" s="18" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C50" s="18" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2043,17 +2080,17 @@
         <v>43</v>
       </c>
       <c r="C52" s="18" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C53" s="18" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C54" s="18" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2062,7 +2099,7 @@
         <v>45</v>
       </c>
       <c r="C56" s="18" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2071,7 +2108,7 @@
         <v>46</v>
       </c>
       <c r="C58" s="18" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2080,26 +2117,26 @@
         <v>47</v>
       </c>
       <c r="C60" s="18" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B62" s="17" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C62" s="18" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C63" s="18" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C64" s="18" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2108,50 +2145,69 @@
         <v>49</v>
       </c>
       <c r="C66" s="18" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="58" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C67" s="20" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C68" s="18" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="47" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C69" s="20" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C70" s="18" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C72" s="18" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C73" s="18" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C74" s="18" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B76" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="C76" s="18" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C77" s="18" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C78" s="18" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C79" s="18" t="s">
+        <v>110</v>
+      </c>
+    </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2258,7 +2314,7 @@
     <hyperlink ref="C39" r:id="rId7" display="Wrote email to Chelsea Finn (cbfinn@eecs.berkeley.edu) → asking about the source code to its paper “One-Shot Imitation from Observing Humans via Domain-Adaptive Meta-Learning”"/>
     <hyperlink ref="C41" r:id="rId8" display="Got response from Chelsea Finn → The code can be found at their github https://github.com/tianheyu927/mil"/>
     <hyperlink ref="C47" r:id="rId9" display="made tutorial on object recognition using the VGG dataset https://machinelearningmastery.com/use-pre-trained-vgg-model-classify-objects-photographs/"/>
-    <hyperlink ref="C62" r:id="rId10" display="https://medium.com/@manivannan_data/how-to-train-yolov3-to-detect-custom-objects-ccbcafeb13d2"/>
+    <hyperlink ref="C62" r:id="rId10" display="Tutorial on “Training YOLOv3 to detect custom objects” (https://medium.com/@manivannan_data/how-to-train-yolov3-to-detect-custom-objects-ccbcafeb13d2)"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -2296,45 +2352,45 @@
   <sheetData>
     <row r="1" customFormat="false" ht="36.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B1" s="23" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="C1" s="23"/>
       <c r="D1" s="23"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="24" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="C3" s="24" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="D3" s="25" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="D4" s="26"/>
     </row>
     <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2431,7 +2487,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="32" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="2" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="C1" s="19"/>
       <c r="D1" s="19"/>
@@ -2442,13 +2498,13 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C2" s="27" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="D2" s="28" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="E2" s="28" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2504,7 +2560,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="32" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="2" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="C1" s="19"/>
       <c r="D1" s="19"/>
@@ -2517,31 +2573,31 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="11" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="G3" s="33" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="H3" s="34" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="I3" s="34" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="J3" s="34" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2742,7 +2798,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="32" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="2" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="C1" s="19"/>
       <c r="D1" s="19"/>
@@ -2754,28 +2810,28 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="11" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="F3" s="33" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="G3" s="34" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="H3" s="34" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="I3" s="48" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2837,7 +2893,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="32" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="2" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="C1" s="19"/>
     </row>
@@ -2846,10 +2902,10 @@
     </row>
     <row r="3" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="11" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
added time stamp for 17.09.
</commit_message>
<xml_diff>
--- a/documentation/Protocol_Timesheet_Todo.xlsx
+++ b/documentation/Protocol_Timesheet_Todo.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Time Sheet" sheetId="1" state="visible" r:id="rId2"/>
@@ -51,6 +51,8 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Time Sheet'!$7:$7</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Time Sheet'!$7:$7</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Time Sheet'!$7:$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Time Sheet'!$7:$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Time Sheet'!$7:$7</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="ColumnTitle1" vbProcedure="false">TimeSheet[[#Headers],[Date(s)]]</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">Protocol!$B$3:$C$3</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">'Project Plan'!$B$3:$D$3</definedName>
@@ -72,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="136">
   <si>
     <t xml:space="preserve">Time Sheet</t>
   </si>
@@ -227,6 +229,9 @@
   </si>
   <si>
     <t xml:space="preserve">14.09.2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17.09.2018</t>
   </si>
   <si>
     <t xml:space="preserve">Protocol</t>
@@ -414,6 +419,9 @@
   </si>
   <si>
     <t xml:space="preserve">--&gt; need to convert the coordinates of an object from the Kinect to the robot positions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Searched for ways how to publish images via a ROS message</t>
   </si>
   <si>
     <t xml:space="preserve">TODO</t>
@@ -1064,10 +1072,10 @@
     <tabColor rgb="FF273645"/>
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="B1:I29"/>
+  <dimension ref="B1:I30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H29" activeCellId="0" sqref="H29"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G30" activeCellId="0" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1144,7 +1152,7 @@
       </c>
       <c r="C6" s="10" t="n">
         <f aca="false">SUBTOTAL(109,TimeSheet[Hours Worked])</f>
-        <v>156.25</v>
+        <v>163.5</v>
       </c>
       <c r="D6" s="10" t="n">
         <f aca="false">IFERROR(IF(C6&lt;=WorkweekHours,C6,WorkweekHours),"")</f>
@@ -1152,7 +1160,7 @@
       </c>
       <c r="E6" s="10" t="n">
         <f aca="false">IFERROR(C6-D6, "")</f>
-        <v>121.25</v>
+        <v>128.5</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="40" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1684,9 +1692,30 @@
         <v>8.25</v>
       </c>
     </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B30" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="C30" s="16" t="n">
+        <v>0.364583333333333</v>
+      </c>
+      <c r="D30" s="16" t="n">
+        <v>0.541666666666667</v>
+      </c>
+      <c r="E30" s="16" t="n">
+        <v>0.5625</v>
+      </c>
+      <c r="F30" s="16" t="n">
+        <v>0.6875</v>
+      </c>
+      <c r="G30" s="15" t="n">
+        <f aca="false">IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Lunch End]]+TimeSheet[[#This Row],[Lunch Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
+        <v>7.25000000000001</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="25">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C1:AMJ1 A2:A9 F2:AMJ2 D3:AMJ4 F5:AMJ6 H7:AMJ7 B8:AMJ9 G10:G29" type="none">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C1:AMJ1 A2:A9 F2:AMJ2 D3:AMJ4 F5:AMJ6 H7:AMJ7 B8:AMJ9 G10:G30" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -1808,10 +1837,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:H80"/>
+  <dimension ref="B1:H82"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C80" activeCellId="0" sqref="C80"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C82" activeCellId="0" sqref="C82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1826,7 +1855,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="32" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C1" s="19"/>
       <c r="D1" s="19"/>
@@ -1837,7 +1866,7 @@
     </row>
     <row r="3" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="11" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C3" s="11" t="s">
         <v>17</v>
@@ -1845,24 +1874,24 @@
     </row>
     <row r="4" s="17" customFormat="true" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="17" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" s="17" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="6" s="17" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="17" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C7" s="17" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1871,32 +1900,32 @@
         <v>26</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C10" s="18" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C11" s="18" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C12" s="18" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="18" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C14" s="18" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1905,7 +1934,7 @@
         <v>28</v>
       </c>
       <c r="C16" s="18" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1924,22 +1953,22 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C20" s="18" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C21" s="18" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C22" s="18" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C23" s="18" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1948,17 +1977,17 @@
         <v>31</v>
       </c>
       <c r="C25" s="18" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C26" s="18" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C27" s="18" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1967,17 +1996,17 @@
         <v>33</v>
       </c>
       <c r="C29" s="18" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C30" s="18" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C31" s="18" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1986,27 +2015,27 @@
         <v>35</v>
       </c>
       <c r="C33" s="18" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C34" s="18" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C35" s="18" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C36" s="18" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C37" s="18" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2018,7 +2047,7 @@
         <v>37</v>
       </c>
       <c r="C39" s="18" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2027,37 +2056,37 @@
         <v>38</v>
       </c>
       <c r="C41" s="18" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C42" s="18" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C43" s="18" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C44" s="18" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C45" s="18" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C46" s="18" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C47" s="18" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2066,12 +2095,12 @@
         <v>41</v>
       </c>
       <c r="C49" s="18" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C50" s="18" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2080,17 +2109,17 @@
         <v>43</v>
       </c>
       <c r="C52" s="18" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C53" s="18" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C54" s="18" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2099,7 +2128,7 @@
         <v>45</v>
       </c>
       <c r="C56" s="18" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2108,7 +2137,7 @@
         <v>46</v>
       </c>
       <c r="C58" s="18" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2117,26 +2146,26 @@
         <v>47</v>
       </c>
       <c r="C60" s="18" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B62" s="17" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C62" s="18" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C63" s="18" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C64" s="18" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2145,43 +2174,43 @@
         <v>49</v>
       </c>
       <c r="C66" s="18" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="58" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C67" s="20" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C68" s="18" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="47" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C69" s="20" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C70" s="18" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C72" s="18" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C73" s="18" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C74" s="18" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2190,26 +2219,33 @@
         <v>50</v>
       </c>
       <c r="C76" s="18" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C77" s="18" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C78" s="18" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C79" s="18" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B81" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="C81" s="18" t="s">
+        <v>112</v>
+      </c>
+    </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2352,45 +2388,45 @@
   <sheetData>
     <row r="1" customFormat="false" ht="36.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B1" s="23" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C1" s="23"/>
       <c r="D1" s="23"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="24" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="C3" s="24" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D3" s="25" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="D4" s="26"/>
     </row>
     <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="C6" s="0" t="s">
         <v>117</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2487,7 +2523,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="32" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="2" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="C1" s="19"/>
       <c r="D1" s="19"/>
@@ -2498,13 +2534,13 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C2" s="27" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="D2" s="28" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="E2" s="28" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2560,7 +2596,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="32" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="2" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="C1" s="19"/>
       <c r="D1" s="19"/>
@@ -2573,31 +2609,31 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="11" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="G3" s="33" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="H3" s="34" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="I3" s="34" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="J3" s="34" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2798,7 +2834,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="32" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="2" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="C1" s="19"/>
       <c r="D1" s="19"/>
@@ -2810,28 +2846,28 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="11" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="F3" s="33" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="G3" s="34" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="H3" s="34" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="I3" s="48" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2893,7 +2929,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="32" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="2" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C1" s="19"/>
     </row>
@@ -2902,10 +2938,10 @@
     </row>
     <row r="3" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="11" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
added timestamp for 21.09.
</commit_message>
<xml_diff>
--- a/documentation/Protocol_Timesheet_Todo.xlsx
+++ b/documentation/Protocol_Timesheet_Todo.xlsx
@@ -53,6 +53,11 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Time Sheet'!$7:$7</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Time Sheet'!$7:$7</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Time Sheet'!$7:$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Time Sheet'!$7:$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Time Sheet'!$7:$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Time Sheet'!$7:$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Time Sheet'!$7:$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Time Sheet'!$7:$7</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="ColumnTitle1" vbProcedure="false">TimeSheet[[#Headers],[Date(s)]]</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">Protocol!$B$3:$C$3</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">'Project Plan'!$B$3:$D$3</definedName>
@@ -74,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="168">
   <si>
     <t xml:space="preserve">Time Sheet</t>
   </si>
@@ -232,6 +237,18 @@
   </si>
   <si>
     <t xml:space="preserve">17.09.2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18.09.2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19.09.2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20.09.2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21.09.2018</t>
   </si>
   <si>
     <t xml:space="preserve">Protocol</t>
@@ -422,6 +439,119 @@
   </si>
   <si>
     <t xml:space="preserve">Searched for ways how to publish images via a ROS message</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Took 150 pictures of the robot hand → 50 with the on-head kinect (256x144), 50 with the front-kinect (256x144) and 50 with the smartphone (320x240)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Training is not converging after 17h→ Avg IOU around 0.8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">did create files hand-yolov3_100.weights to hand-yolov3_30000.weights</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Network settings (hand-yolov3.cfg):</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[net]
+# Testing
+# batch=1
+# subdivisions=1
+# Training
+batch=10
+subdivisions=8
+width=608
+height=608
+channels=3
+momentum=0.9
+decay=0.0005
+angle=0
+saturation = 1.5
+exposure = 1.5
+hue=.1
+learning_rate=0.001
+burn_in=1000
+max_batches = 500200
+policy=steps
+steps=400000,450000
+scales=.1,.1
+[convolutional]
+batch_normalize=1
+filters=32
+size=3
+stride=1
+pad=1
+activation=leaky
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Testing the weights → Problem with OpenCV version (https://github.com/pjreddie/darknet/issues/518)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">installed older OpenCV version like here (https://github.com/madhawav/YOLO3-4-Py/blob/master/tools/install_opencv34.sh)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This was not a good idea → did the installation of OpenCV 3.4.3 again (https://www.pyimagesearch.com/2018/05/28/ubuntu-18-04-how-to-install-opencv/)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Back on newest OpenCV version</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Followed this (https://www.learnopencv.com/install-opencv3-on-ubuntu/) tutorial to install OpenCV 3.4.0 → pay attention to git checkout</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Same error → ImportError: /usr/local/lib/python2.7/dist-packages/cv2.so: undefined symbol: _ZTIN2cv3dnn19experimental_dnn_v35LayerE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">upgraded back to 3.4.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">removed opencv with sudo make uninstall and then removed the folders with rm -rf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">also removed the cv.so files in dist-packages and site-packages</t>
+  </si>
+  <si>
+    <t xml:space="preserve">added export PKG_CONFIG_PATH=$PKG_CONFIG_PATH:/usr/lib/pkgconfig to bashrc → same error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">adapted opencv_yolo code </t>
+  </si>
+  <si>
+    <t xml:space="preserve">network is detecting objects but the trained weights did not work</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pedro proposed I should have a look at the weights files to see if there was a problem saving the weights</t>
+  </si>
+  <si>
+    <t xml:space="preserve">weight files can not be opened easily → they are binary files</t>
+  </si>
+  <si>
+    <t xml:space="preserve">this is discussed on https://groups.google.com/forum/#!topic/darknet/ZiNcHN37NTY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">found the program on https://twitter.com/genekogan/status/852111806218752000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tried to clone the repository and run the visualization but it did not work</t>
+  </si>
+  <si>
+    <t xml:space="preserve">started training with new dataset</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bounding boxes where not working with the OpenCV Yolo code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">--&gt; fixed it</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OpenCV code is now fully working with the COCO dataset on the pretrained yolo weights</t>
+  </si>
+  <si>
+    <t xml:space="preserve">training stopped at iteration 15730 with the CUDA Error: out of memory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the newly trained weights (used the one with 10000 iterations) for detecting the sawyer hand is not detecting anything</t>
   </si>
   <si>
     <t xml:space="preserve">TODO</t>
@@ -498,10 +628,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="10">
-    <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="0.00"/>
-    <numFmt numFmtId="166" formatCode="D\-MMM\-YY;@"/>
-    <numFmt numFmtId="167" formatCode="#,##0.00;\-#,##0.00"/>
+    <numFmt numFmtId="164" formatCode="#,##0.00;\-#,##0.00"/>
+    <numFmt numFmtId="165" formatCode="General"/>
+    <numFmt numFmtId="166" formatCode="0.00"/>
+    <numFmt numFmtId="167" formatCode="D\-MMM\-YY;@"/>
     <numFmt numFmtId="168" formatCode="DD\.MM\.YY"/>
     <numFmt numFmtId="169" formatCode="H:MM:SS;@"/>
     <numFmt numFmtId="170" formatCode="HH:MM:SS"/>
@@ -603,7 +733,7 @@
     </border>
   </borders>
   <cellStyleXfs count="21">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -626,24 +756,20 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="167" fontId="7" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="49">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -651,31 +777,31 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -683,6 +809,10 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -691,7 +821,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -699,7 +829,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -723,11 +853,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -743,7 +873,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -775,7 +905,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -783,7 +913,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -795,7 +925,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -803,7 +933,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -811,11 +941,11 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -837,90 +967,70 @@
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
     <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="5">
     <dxf>
+      <font>
+        <name val="Calibri"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <color rgb="FF000000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Calibri"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <color rgb="FF000000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Calibri"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <color rgb="FF273645"/>
+        <u val="none"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="#,##0.00;\-#,##0.00"/>
       <fill>
         <patternFill>
-          <bgColor rgb="FFC93737"/>
+          <bgColor rgb="FFFFFFFF"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <name val="Calibri"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <color rgb="FF273645"/>
+        <u val="none"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="#,##0.00;\-#,##0.00"/>
       <fill>
         <patternFill>
-          <bgColor rgb="FF58CC7C"/>
+          <bgColor rgb="FFFFFFFF"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC93737"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF58CC7C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC93737"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF58CC7C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC93737"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF58CC7C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC93737"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF58CC7C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC93737"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF58CC7C"/>
-        </patternFill>
-      </fill>
+      <font>
+        <name val="Calibri"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <color rgb="FF000000"/>
+      </font>
     </dxf>
   </dxfs>
   <colors>
@@ -966,7 +1076,7 @@
       <rgbColor rgb="FFCC99FF"/>
       <rgbColor rgb="FFFFCC99"/>
       <rgbColor rgb="FF3366FF"/>
-      <rgbColor rgb="FF58CC7C"/>
+      <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
@@ -978,7 +1088,7 @@
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
       <rgbColor rgb="FF993300"/>
-      <rgbColor rgb="FFC93737"/>
+      <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF273645"/>
     </indexedColors>
@@ -1072,10 +1182,10 @@
     <tabColor rgb="FF273645"/>
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="B1:I30"/>
+  <dimension ref="B1:I34"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G30" activeCellId="0" sqref="G30"/>
+      <selection pane="topLeft" activeCell="E34" activeCellId="0" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1152,7 +1262,7 @@
       </c>
       <c r="C6" s="10" t="n">
         <f aca="false">SUBTOTAL(109,TimeSheet[Hours Worked])</f>
-        <v>163.5</v>
+        <v>189.5</v>
       </c>
       <c r="D6" s="10" t="n">
         <f aca="false">IFERROR(IF(C6&lt;=WorkweekHours,C6,WorkweekHours),"")</f>
@@ -1160,7 +1270,7 @@
       </c>
       <c r="E6" s="10" t="n">
         <f aca="false">IFERROR(C6-D6, "")</f>
-        <v>128.5</v>
+        <v>154.5</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="40" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1713,9 +1823,83 @@
         <v>7.25000000000001</v>
       </c>
     </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B31" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="C31" s="16" t="n">
+        <v>0.395833333333333</v>
+      </c>
+      <c r="D31" s="16" t="n">
+        <v>0.541666666666667</v>
+      </c>
+      <c r="E31" s="16" t="n">
+        <v>0.572916666666667</v>
+      </c>
+      <c r="F31" s="16" t="n">
+        <v>0.791666666666667</v>
+      </c>
+      <c r="G31" s="15" t="n">
+        <f aca="false">IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Lunch End]]+TimeSheet[[#This Row],[Lunch Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
+        <v>8.75</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B32" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="C32" s="16" t="n">
+        <v>0.385416666666667</v>
+      </c>
+      <c r="D32" s="16" t="n">
+        <v>0.510416666666667</v>
+      </c>
+      <c r="E32" s="16" t="n">
+        <v>0.552083333333333</v>
+      </c>
+      <c r="F32" s="16" t="n">
+        <v>0.791666666666667</v>
+      </c>
+      <c r="G32" s="15" t="n">
+        <f aca="false">IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Lunch End]]+TimeSheet[[#This Row],[Lunch Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
+        <v>8.74999999999999</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B33" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="C33" s="16" t="n">
+        <v>0.385416666666667</v>
+      </c>
+      <c r="D33" s="16" t="n">
+        <v>0.541666666666667</v>
+      </c>
+      <c r="E33" s="16" t="n">
+        <v>0.572916666666667</v>
+      </c>
+      <c r="F33" s="16" t="n">
+        <v>0.770833333333333</v>
+      </c>
+      <c r="G33" s="15" t="n">
+        <f aca="false">IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Lunch End]]+TimeSheet[[#This Row],[Lunch Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B34" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="C34" s="16" t="n">
+        <v>0.395833333333333</v>
+      </c>
+      <c r="D34" s="16" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="25">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C1:AMJ1 A2:A9 F2:AMJ2 D3:AMJ4 F5:AMJ6 H7:AMJ7 B8:AMJ9 G10:G30" type="none">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C1:AMJ1 A2:A9 F2:AMJ2 D3:AMJ4 F5:AMJ6 H7:AMJ7 B8:AMJ9 G10:G33" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -1837,10 +2021,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:H82"/>
+  <dimension ref="B1:H115"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C82" activeCellId="0" sqref="C82"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A61" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C115" activeCellId="0" sqref="C115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1855,7 +2039,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="32" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="2" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="C1" s="19"/>
       <c r="D1" s="19"/>
@@ -1866,7 +2050,7 @@
     </row>
     <row r="3" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="11" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="C3" s="11" t="s">
         <v>17</v>
@@ -1874,24 +2058,24 @@
     </row>
     <row r="4" s="17" customFormat="true" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="17" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" s="17" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="6" s="17" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="17" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C7" s="17" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1900,32 +2084,32 @@
         <v>26</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C10" s="18" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C11" s="18" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C12" s="18" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="18" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C14" s="18" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1934,7 +2118,7 @@
         <v>28</v>
       </c>
       <c r="C16" s="18" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1953,22 +2137,22 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C20" s="18" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C21" s="18" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C22" s="18" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C23" s="18" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1977,17 +2161,17 @@
         <v>31</v>
       </c>
       <c r="C25" s="18" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C26" s="18" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C27" s="18" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1996,17 +2180,17 @@
         <v>33</v>
       </c>
       <c r="C29" s="18" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C30" s="18" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C31" s="18" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2015,27 +2199,27 @@
         <v>35</v>
       </c>
       <c r="C33" s="18" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C34" s="18" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C35" s="18" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C36" s="18" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C37" s="18" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2047,7 +2231,7 @@
         <v>37</v>
       </c>
       <c r="C39" s="18" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2056,37 +2240,37 @@
         <v>38</v>
       </c>
       <c r="C41" s="18" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C42" s="18" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C43" s="18" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C44" s="18" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C45" s="18" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C46" s="18" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C47" s="18" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2095,12 +2279,12 @@
         <v>41</v>
       </c>
       <c r="C49" s="18" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C50" s="18" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2109,17 +2293,17 @@
         <v>43</v>
       </c>
       <c r="C52" s="18" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C53" s="18" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C54" s="18" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2128,7 +2312,7 @@
         <v>45</v>
       </c>
       <c r="C56" s="18" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2137,7 +2321,7 @@
         <v>46</v>
       </c>
       <c r="C58" s="18" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2146,26 +2330,26 @@
         <v>47</v>
       </c>
       <c r="C60" s="18" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B62" s="17" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="C62" s="18" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C63" s="18" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C64" s="18" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2174,43 +2358,43 @@
         <v>49</v>
       </c>
       <c r="C66" s="18" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="58" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C67" s="20" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C68" s="18" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="47" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C69" s="20" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C70" s="18" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C72" s="18" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C73" s="18" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C74" s="18" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2219,22 +2403,22 @@
         <v>50</v>
       </c>
       <c r="C76" s="18" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C77" s="18" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C78" s="18" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C79" s="18" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2243,42 +2427,166 @@
         <v>51</v>
       </c>
       <c r="C81" s="18" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B83" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="C83" s="18" t="s">
+        <v>117</v>
+      </c>
+    </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B85" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="C85" s="18" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C86" s="18" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C87" s="0" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="43" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C88" s="20" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C89" s="18" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C90" s="18" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C91" s="18" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C92" s="18" t="s">
+        <v>125</v>
+      </c>
+    </row>
     <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C94" s="18" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C95" s="18" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C96" s="18" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C97" s="18" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C98" s="18" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C99" s="18" t="s">
+        <v>131</v>
+      </c>
+    </row>
     <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B101" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="C101" s="18" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C102" s="18" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C103" s="18" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C104" s="18" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C105" s="18" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C106" s="18" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C107" s="18" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C108" s="18" t="s">
+        <v>139</v>
+      </c>
+    </row>
     <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B110" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="C110" s="18" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C111" s="18" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C112" s="18" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C113" s="0" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C114" s="18" t="s">
+        <v>144</v>
+      </c>
+    </row>
     <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2351,6 +2659,12 @@
     <hyperlink ref="C41" r:id="rId8" display="Got response from Chelsea Finn → The code can be found at their github https://github.com/tianheyu927/mil"/>
     <hyperlink ref="C47" r:id="rId9" display="made tutorial on object recognition using the VGG dataset https://machinelearningmastery.com/use-pre-trained-vgg-model-classify-objects-photographs/"/>
     <hyperlink ref="C62" r:id="rId10" display="Tutorial on “Training YOLOv3 to detect custom objects” (https://medium.com/@manivannan_data/how-to-train-yolov3-to-detect-custom-objects-ccbcafeb13d2)"/>
+    <hyperlink ref="C89" r:id="rId11" display="Testing the weights → Problem with OpenCV version (https://github.com/pjreddie/darknet/issues/518)"/>
+    <hyperlink ref="C90" r:id="rId12" display="installed older OpenCV version like here (https://github.com/madhawav/YOLO3-4-Py/blob/master/tools/install_opencv34.sh)"/>
+    <hyperlink ref="C91" r:id="rId13" display="This was not a good idea → did the installation of OpenCV 3.4.3 again (https://www.pyimagesearch.com/2018/05/28/ubuntu-18-04-how-to-install-opencv/)"/>
+    <hyperlink ref="C94" r:id="rId14" display="Followed this (https://www.learnopencv.com/install-opencv3-on-ubuntu/) tutorial to install OpenCV 3.4.0 → pay attention to git checkout"/>
+    <hyperlink ref="C105" r:id="rId15" location="!topic/darknet/ZiNcHN37NTY" display="this is discussed on https://groups.google.com/forum/#!topic/darknet/ZiNcHN37NTY"/>
+    <hyperlink ref="C106" r:id="rId16" display="found the program on https://twitter.com/genekogan/status/852111806218752000"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -2360,7 +2674,7 @@
     <oddFooter/>
   </headerFooter>
   <tableParts>
-    <tablePart r:id="rId11"/>
+    <tablePart r:id="rId17"/>
   </tableParts>
 </worksheet>
 </file>
@@ -2388,45 +2702,45 @@
   <sheetData>
     <row r="1" customFormat="false" ht="36.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B1" s="23" t="s">
-        <v>113</v>
+        <v>145</v>
       </c>
       <c r="C1" s="23"/>
       <c r="D1" s="23"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="24" t="s">
-        <v>114</v>
+        <v>146</v>
       </c>
       <c r="C3" s="24" t="s">
-        <v>115</v>
+        <v>147</v>
       </c>
       <c r="D3" s="25" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>116</v>
+        <v>148</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>117</v>
+        <v>149</v>
       </c>
       <c r="D4" s="26"/>
     </row>
     <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="s">
-        <v>118</v>
+        <v>150</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>117</v>
+        <v>149</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
-        <v>119</v>
+        <v>151</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>117</v>
+        <v>149</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2464,27 +2778,27 @@
   </sheetData>
   <conditionalFormatting sqref="C2:C14 C16 C18 C29:C1048576 C27 C20:C24">
     <cfRule type="containsText" priority="2" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="no" dxfId="0"/>
-    <cfRule type="containsText" priority="3" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="yes" dxfId="1"/>
+    <cfRule type="containsText" priority="3" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="yes" dxfId="0"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19">
-    <cfRule type="containsText" priority="4" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="no" dxfId="2"/>
-    <cfRule type="containsText" priority="5" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="yes" dxfId="3"/>
+    <cfRule type="containsText" priority="4" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="no" dxfId="0"/>
+    <cfRule type="containsText" priority="5" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="yes" dxfId="0"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28">
-    <cfRule type="containsText" priority="6" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="no" dxfId="4"/>
-    <cfRule type="containsText" priority="7" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="yes" dxfId="5"/>
+    <cfRule type="containsText" priority="6" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="no" dxfId="0"/>
+    <cfRule type="containsText" priority="7" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="yes" dxfId="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C17">
-    <cfRule type="containsText" priority="8" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="no" dxfId="6"/>
-    <cfRule type="containsText" priority="9" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="yes" dxfId="7"/>
+    <cfRule type="containsText" priority="8" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="no" dxfId="1"/>
+    <cfRule type="containsText" priority="9" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="yes" dxfId="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26">
-    <cfRule type="containsText" priority="10" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="no" dxfId="8"/>
-    <cfRule type="containsText" priority="11" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="yes" dxfId="9"/>
+    <cfRule type="containsText" priority="10" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="no" dxfId="2"/>
+    <cfRule type="containsText" priority="11" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="yes" dxfId="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C25">
-    <cfRule type="containsText" priority="12" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="no" dxfId="10"/>
-    <cfRule type="containsText" priority="13" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="yes" dxfId="11"/>
+    <cfRule type="containsText" priority="12" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="no" dxfId="3"/>
+    <cfRule type="containsText" priority="13" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="yes" dxfId="4"/>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -2523,7 +2837,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="32" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="2" t="s">
-        <v>120</v>
+        <v>152</v>
       </c>
       <c r="C1" s="19"/>
       <c r="D1" s="19"/>
@@ -2534,13 +2848,13 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C2" s="27" t="s">
-        <v>121</v>
+        <v>153</v>
       </c>
       <c r="D2" s="28" t="s">
-        <v>122</v>
+        <v>154</v>
       </c>
       <c r="E2" s="28" t="s">
-        <v>123</v>
+        <v>155</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2596,7 +2910,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="32" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="2" t="s">
-        <v>124</v>
+        <v>156</v>
       </c>
       <c r="C1" s="19"/>
       <c r="D1" s="19"/>
@@ -2609,31 +2923,31 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="11" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>125</v>
+        <v>157</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>126</v>
+        <v>158</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>127</v>
+        <v>159</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>128</v>
+        <v>160</v>
       </c>
       <c r="G3" s="33" t="s">
-        <v>129</v>
+        <v>161</v>
       </c>
       <c r="H3" s="34" t="s">
-        <v>130</v>
+        <v>162</v>
       </c>
       <c r="I3" s="34" t="s">
-        <v>131</v>
+        <v>163</v>
       </c>
       <c r="J3" s="34" t="s">
-        <v>132</v>
+        <v>164</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2834,7 +3148,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="32" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="2" t="s">
-        <v>133</v>
+        <v>165</v>
       </c>
       <c r="C1" s="19"/>
       <c r="D1" s="19"/>
@@ -2846,28 +3160,28 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="11" t="s">
-        <v>125</v>
+        <v>157</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>126</v>
+        <v>158</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>127</v>
+        <v>159</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>128</v>
+        <v>160</v>
       </c>
       <c r="F3" s="33" t="s">
-        <v>129</v>
+        <v>161</v>
       </c>
       <c r="G3" s="34" t="s">
-        <v>130</v>
+        <v>162</v>
       </c>
       <c r="H3" s="34" t="s">
-        <v>131</v>
+        <v>163</v>
       </c>
       <c r="I3" s="48" t="s">
-        <v>132</v>
+        <v>164</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2929,7 +3243,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="32" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="2" t="s">
-        <v>134</v>
+        <v>166</v>
       </c>
       <c r="C1" s="19"/>
     </row>
@@ -2938,10 +3252,10 @@
     </row>
     <row r="3" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="11" t="s">
-        <v>114</v>
+        <v>146</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>135</v>
+        <v>167</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
added timestamp for 24.09.
</commit_message>
<xml_diff>
--- a/documentation/Protocol_Timesheet_Todo.xlsx
+++ b/documentation/Protocol_Timesheet_Todo.xlsx
@@ -58,6 +58,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Time Sheet'!$7:$7</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Time Sheet'!$7:$7</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Time Sheet'!$7:$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Time Sheet'!$7:$7</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="ColumnTitle1" vbProcedure="false">TimeSheet[[#Headers],[Date(s)]]</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">Protocol!$B$3:$C$3</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">'Project Plan'!$B$3:$D$3</definedName>
@@ -79,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="171">
   <si>
     <t xml:space="preserve">Time Sheet</t>
   </si>
@@ -249,6 +250,9 @@
   </si>
   <si>
     <t xml:space="preserve">21.09.2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24.09.2018</t>
   </si>
   <si>
     <t xml:space="preserve">Protocol</t>
@@ -552,6 +556,12 @@
   </si>
   <si>
     <t xml:space="preserve">the newly trained weights (used the one with 10000 iterations) for detecting the sawyer hand is not detecting anything</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coco dataset has got 82783 images for </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deleted 46 images from the 500 images where there was no hand on it</t>
   </si>
   <si>
     <t xml:space="preserve">TODO</t>
@@ -967,22 +977,27 @@
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
     <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="4">
     <dxf>
       <font>
         <name val="Calibri"/>
         <charset val="1"/>
         <family val="2"/>
-        <color rgb="FF000000"/>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <color rgb="FF273645"/>
+        <u val="none"/>
       </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
+      <numFmt numFmtId="164" formatCode="#,##0.00;\-#,##0.00"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="00FFFFFF"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </dxf>
     <dxf>
       <font>
@@ -1000,9 +1015,10 @@
       <numFmt numFmtId="164" formatCode="#,##0.00;\-#,##0.00"/>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFFFFF"/>
+          <bgColor rgb="00FFFFFF"/>
         </patternFill>
       </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </dxf>
     <dxf>
       <font>
@@ -1020,17 +1036,31 @@
       <numFmt numFmtId="164" formatCode="#,##0.00;\-#,##0.00"/>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFFFFF"/>
+          <bgColor rgb="00FFFFFF"/>
         </patternFill>
       </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </dxf>
     <dxf>
       <font>
         <name val="Calibri"/>
         <charset val="1"/>
         <family val="2"/>
-        <color rgb="FF000000"/>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <color rgb="FF273645"/>
+        <u val="none"/>
       </font>
+      <numFmt numFmtId="164" formatCode="#,##0.00;\-#,##0.00"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="00FFFFFF"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </dxf>
   </dxfs>
   <colors>
@@ -1182,10 +1212,10 @@
     <tabColor rgb="FF273645"/>
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="B1:I34"/>
+  <dimension ref="B1:I35"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E34" activeCellId="0" sqref="E34"/>
+      <selection pane="topLeft" activeCell="D35" activeCellId="0" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1895,6 +1925,14 @@
       </c>
       <c r="D34" s="16" t="n">
         <v>0.5</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B35" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="C35" s="16" t="n">
+        <v>0.395833333333333</v>
       </c>
     </row>
   </sheetData>
@@ -2021,10 +2059,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:H115"/>
+  <dimension ref="B1:H118"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A61" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C115" activeCellId="0" sqref="C115"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A70" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C118" activeCellId="0" sqref="C118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2039,7 +2077,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="32" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C1" s="19"/>
       <c r="D1" s="19"/>
@@ -2050,7 +2088,7 @@
     </row>
     <row r="3" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="11" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C3" s="11" t="s">
         <v>17</v>
@@ -2058,24 +2096,24 @@
     </row>
     <row r="4" s="17" customFormat="true" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="17" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" s="17" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="6" s="17" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="17" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C7" s="17" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2084,32 +2122,32 @@
         <v>26</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C10" s="18" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C11" s="18" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C12" s="18" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="18" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C14" s="18" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2118,7 +2156,7 @@
         <v>28</v>
       </c>
       <c r="C16" s="18" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2137,22 +2175,22 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C20" s="18" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C21" s="18" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C22" s="18" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C23" s="18" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2161,17 +2199,17 @@
         <v>31</v>
       </c>
       <c r="C25" s="18" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C26" s="18" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C27" s="18" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2180,17 +2218,17 @@
         <v>33</v>
       </c>
       <c r="C29" s="18" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C30" s="18" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C31" s="18" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2199,27 +2237,27 @@
         <v>35</v>
       </c>
       <c r="C33" s="18" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C34" s="18" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C35" s="18" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C36" s="18" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C37" s="18" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2231,7 +2269,7 @@
         <v>37</v>
       </c>
       <c r="C39" s="18" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2240,37 +2278,37 @@
         <v>38</v>
       </c>
       <c r="C41" s="18" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C42" s="18" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C43" s="18" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C44" s="18" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C45" s="18" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C46" s="18" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C47" s="18" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2279,12 +2317,12 @@
         <v>41</v>
       </c>
       <c r="C49" s="18" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C50" s="18" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2293,17 +2331,17 @@
         <v>43</v>
       </c>
       <c r="C52" s="18" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C53" s="18" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C54" s="18" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2312,7 +2350,7 @@
         <v>45</v>
       </c>
       <c r="C56" s="18" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2321,7 +2359,7 @@
         <v>46</v>
       </c>
       <c r="C58" s="18" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2330,26 +2368,26 @@
         <v>47</v>
       </c>
       <c r="C60" s="18" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B62" s="17" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C62" s="18" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C63" s="18" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C64" s="18" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2358,43 +2396,43 @@
         <v>49</v>
       </c>
       <c r="C66" s="18" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="58" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C67" s="20" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C68" s="18" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="47" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C69" s="20" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C70" s="18" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C72" s="18" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C73" s="18" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C74" s="18" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2403,22 +2441,22 @@
         <v>50</v>
       </c>
       <c r="C76" s="18" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C77" s="18" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C78" s="18" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C79" s="18" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2427,7 +2465,7 @@
         <v>51</v>
       </c>
       <c r="C81" s="18" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2436,7 +2474,7 @@
         <v>52</v>
       </c>
       <c r="C83" s="18" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2445,73 +2483,73 @@
         <v>53</v>
       </c>
       <c r="C85" s="18" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C86" s="18" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C87" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="43" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C88" s="20" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C89" s="18" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C90" s="18" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C91" s="18" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C92" s="18" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C94" s="18" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C95" s="18" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C96" s="18" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C97" s="18" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C98" s="18" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C99" s="18" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2520,42 +2558,42 @@
         <v>54</v>
       </c>
       <c r="C101" s="18" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C102" s="18" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C103" s="18" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C104" s="18" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C105" s="18" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C106" s="18" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C107" s="18" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C108" s="18" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2564,32 +2602,43 @@
         <v>55</v>
       </c>
       <c r="C110" s="18" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C111" s="18" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C112" s="18" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C113" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C114" s="18" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B116" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="C116" s="18" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C117" s="18" t="s">
+        <v>147</v>
+      </c>
+    </row>
     <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2702,45 +2751,45 @@
   <sheetData>
     <row r="1" customFormat="false" ht="36.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B1" s="23" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="C1" s="23"/>
       <c r="D1" s="23"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="24" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="C3" s="24" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="D3" s="25" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="D4" s="26"/>
     </row>
     <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2837,7 +2886,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="32" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="2" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="C1" s="19"/>
       <c r="D1" s="19"/>
@@ -2848,13 +2897,13 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C2" s="27" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="D2" s="28" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="E2" s="28" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2910,7 +2959,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="32" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="2" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="C1" s="19"/>
       <c r="D1" s="19"/>
@@ -2923,31 +2972,31 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="11" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="G3" s="33" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="H3" s="34" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="I3" s="34" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="J3" s="34" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3148,7 +3197,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="32" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="2" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="C1" s="19"/>
       <c r="D1" s="19"/>
@@ -3160,28 +3209,28 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="11" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="F3" s="33" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="G3" s="34" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="H3" s="34" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="I3" s="48" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -3243,7 +3292,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="32" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="2" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="C1" s="19"/>
     </row>
@@ -3252,10 +3301,10 @@
     </row>
     <row r="3" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="11" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
added timestamp for 25.09.
</commit_message>
<xml_diff>
--- a/documentation/Protocol_Timesheet_Todo.xlsx
+++ b/documentation/Protocol_Timesheet_Todo.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Time Sheet" sheetId="1" state="visible" r:id="rId2"/>
@@ -59,6 +59,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Time Sheet'!$7:$7</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Time Sheet'!$7:$7</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Time Sheet'!$7:$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Time Sheet'!$7:$7</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="ColumnTitle1" vbProcedure="false">TimeSheet[[#Headers],[Date(s)]]</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">Protocol!$B$3:$C$3</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">'Project Plan'!$B$3:$D$3</definedName>
@@ -80,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="179">
   <si>
     <t xml:space="preserve">Time Sheet</t>
   </si>
@@ -253,6 +254,9 @@
   </si>
   <si>
     <t xml:space="preserve">24.09.2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25.09.2018</t>
   </si>
   <si>
     <t xml:space="preserve">Protocol</t>
@@ -562,6 +566,30 @@
   </si>
   <si>
     <t xml:space="preserve">Deleted 46 images from the 500 images where there was no hand on it</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Did annotation again for the residual images and and tried training again</t>
+  </si>
+  <si>
+    <t xml:space="preserve">error: darknet: ./src/utils.c:256: error: Assertion `0' failed.
+Aborted (core dumped)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">when lowering the batch size or changing the width and height of the network input there is a different error: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resizing
+544
+Floating point exception (core dumped)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Solved floating point exeption → https://groups.google.com/forum/#!topic/darknet/FUDYIrbIz0I</t>
+  </si>
+  <si>
+    <t xml:space="preserve">train and test files where empty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">--names cfg/hand_take2/hand2-obj.names --config cfg/hand_take2/hand2-yolov3.cfg --weights cfg/hand_take2/hand2-yolov3_10000.weights --cam_idx=1</t>
   </si>
   <si>
     <t xml:space="preserve">TODO</t>
@@ -977,7 +1005,7 @@
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
     <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="5">
     <dxf>
       <font>
         <name val="Calibri"/>
@@ -1060,6 +1088,15 @@
           <bgColor rgb="00FFFFFF"/>
         </patternFill>
       </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Calibri"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <color rgb="FF000000"/>
+      </font>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </dxf>
   </dxfs>
@@ -1212,10 +1249,10 @@
     <tabColor rgb="FF273645"/>
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="B1:I35"/>
+  <dimension ref="B1:I36"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D35" activeCellId="0" sqref="D35"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G36" activeCellId="0" sqref="G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1292,7 +1329,7 @@
       </c>
       <c r="C6" s="10" t="n">
         <f aca="false">SUBTOTAL(109,TimeSheet[Hours Worked])</f>
-        <v>189.5</v>
+        <v>215</v>
       </c>
       <c r="D6" s="10" t="n">
         <f aca="false">IFERROR(IF(C6&lt;=WorkweekHours,C6,WorkweekHours),"")</f>
@@ -1300,7 +1337,7 @@
       </c>
       <c r="E6" s="10" t="n">
         <f aca="false">IFERROR(C6-D6, "")</f>
-        <v>154.5</v>
+        <v>180</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="40" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1926,6 +1963,16 @@
       <c r="D34" s="16" t="n">
         <v>0.5</v>
       </c>
+      <c r="E34" s="16" t="n">
+        <v>0.541666666666667</v>
+      </c>
+      <c r="F34" s="16" t="n">
+        <v>0.770833333333333</v>
+      </c>
+      <c r="G34" s="15" t="n">
+        <f aca="false">IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Lunch End]]+TimeSheet[[#This Row],[Lunch Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
+        <v>8.00000000000001</v>
+      </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="0" t="s">
@@ -1934,10 +1981,44 @@
       <c r="C35" s="16" t="n">
         <v>0.395833333333333</v>
       </c>
+      <c r="D35" s="16" t="n">
+        <v>0.5625</v>
+      </c>
+      <c r="E35" s="16" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="F35" s="16" t="n">
+        <v>0.770833333333333</v>
+      </c>
+      <c r="G35" s="15" t="n">
+        <f aca="false">IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Lunch End]]+TimeSheet[[#This Row],[Lunch Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
+        <v>7.50000000000001</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B36" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="C36" s="16" t="n">
+        <v>0.3125</v>
+      </c>
+      <c r="D36" s="16" t="n">
+        <v>0.541666666666667</v>
+      </c>
+      <c r="E36" s="16" t="n">
+        <v>0.5625</v>
+      </c>
+      <c r="F36" s="16" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="G36" s="15" t="n">
+        <f aca="false">IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Lunch End]]+TimeSheet[[#This Row],[Lunch Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
+        <v>10</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="25">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C1:AMJ1 A2:A9 F2:AMJ2 D3:AMJ4 F5:AMJ6 H7:AMJ7 B8:AMJ9 G10:G33" type="none">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C1:AMJ1 A2:A9 F2:AMJ2 D3:AMJ4 F5:AMJ6 H7:AMJ7 B8:AMJ9 G10:G36" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -2059,10 +2140,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:H118"/>
+  <dimension ref="B1:H126"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A70" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C118" activeCellId="0" sqref="C118"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A94" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C126" activeCellId="0" sqref="C126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2077,7 +2158,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="32" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C1" s="19"/>
       <c r="D1" s="19"/>
@@ -2088,7 +2169,7 @@
     </row>
     <row r="3" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="11" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C3" s="11" t="s">
         <v>17</v>
@@ -2096,24 +2177,24 @@
     </row>
     <row r="4" s="17" customFormat="true" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="17" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" s="17" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="6" s="17" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="17" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C7" s="17" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2122,32 +2203,32 @@
         <v>26</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C10" s="18" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C11" s="18" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C12" s="18" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="18" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C14" s="18" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2156,7 +2237,7 @@
         <v>28</v>
       </c>
       <c r="C16" s="18" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2175,22 +2256,22 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C20" s="18" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C21" s="18" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C22" s="18" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C23" s="18" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2199,17 +2280,17 @@
         <v>31</v>
       </c>
       <c r="C25" s="18" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C26" s="18" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C27" s="18" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2218,17 +2299,17 @@
         <v>33</v>
       </c>
       <c r="C29" s="18" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C30" s="18" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C31" s="18" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2237,27 +2318,27 @@
         <v>35</v>
       </c>
       <c r="C33" s="18" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C34" s="18" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C35" s="18" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C36" s="18" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C37" s="18" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2269,7 +2350,7 @@
         <v>37</v>
       </c>
       <c r="C39" s="18" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2278,37 +2359,37 @@
         <v>38</v>
       </c>
       <c r="C41" s="18" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C42" s="18" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C43" s="18" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C44" s="18" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C45" s="18" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C46" s="18" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C47" s="18" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2317,12 +2398,12 @@
         <v>41</v>
       </c>
       <c r="C49" s="18" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C50" s="18" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2331,17 +2412,17 @@
         <v>43</v>
       </c>
       <c r="C52" s="18" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C53" s="18" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C54" s="18" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2350,7 +2431,7 @@
         <v>45</v>
       </c>
       <c r="C56" s="18" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2359,7 +2440,7 @@
         <v>46</v>
       </c>
       <c r="C58" s="18" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2368,26 +2449,26 @@
         <v>47</v>
       </c>
       <c r="C60" s="18" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B62" s="17" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C62" s="18" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C63" s="18" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C64" s="18" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2396,43 +2477,43 @@
         <v>49</v>
       </c>
       <c r="C66" s="18" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="58" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C67" s="20" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C68" s="18" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="47" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C69" s="20" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C70" s="18" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C72" s="18" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C73" s="18" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C74" s="18" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2441,22 +2522,22 @@
         <v>50</v>
       </c>
       <c r="C76" s="18" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C77" s="18" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C78" s="18" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C79" s="18" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2465,7 +2546,7 @@
         <v>51</v>
       </c>
       <c r="C81" s="18" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2474,7 +2555,7 @@
         <v>52</v>
       </c>
       <c r="C83" s="18" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2483,73 +2564,73 @@
         <v>53</v>
       </c>
       <c r="C85" s="18" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C86" s="18" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C87" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="43" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C88" s="20" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C89" s="18" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C90" s="18" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C91" s="18" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C92" s="18" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C94" s="18" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C95" s="18" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C96" s="18" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C97" s="18" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C98" s="18" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C99" s="18" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2558,42 +2639,42 @@
         <v>54</v>
       </c>
       <c r="C101" s="18" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C102" s="18" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C103" s="18" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C104" s="18" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C105" s="18" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C106" s="18" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C107" s="18" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C108" s="18" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2602,27 +2683,27 @@
         <v>55</v>
       </c>
       <c r="C110" s="18" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C111" s="18" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C112" s="18" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C113" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C114" s="18" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2631,22 +2712,53 @@
         <v>56</v>
       </c>
       <c r="C116" s="18" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C117" s="18" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+        <v>148</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C118" s="18" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C119" s="20" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C120" s="18" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="121" customFormat="false" ht="36" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C121" s="20" t="s">
+        <v>152</v>
+      </c>
+    </row>
     <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B123" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="C123" s="18" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C124" s="18" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C125" s="18" t="s">
+        <v>155</v>
+      </c>
+    </row>
     <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2714,6 +2826,7 @@
     <hyperlink ref="C94" r:id="rId14" display="Followed this (https://www.learnopencv.com/install-opencv3-on-ubuntu/) tutorial to install OpenCV 3.4.0 → pay attention to git checkout"/>
     <hyperlink ref="C105" r:id="rId15" location="!topic/darknet/ZiNcHN37NTY" display="this is discussed on https://groups.google.com/forum/#!topic/darknet/ZiNcHN37NTY"/>
     <hyperlink ref="C106" r:id="rId16" display="found the program on https://twitter.com/genekogan/status/852111806218752000"/>
+    <hyperlink ref="C123" r:id="rId17" location="!topic/darknet/FUDYIrbIz0I" display="https://groups.google.com/forum/#!topic/darknet/FUDYIrbIz0I"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -2723,7 +2836,7 @@
     <oddFooter/>
   </headerFooter>
   <tableParts>
-    <tablePart r:id="rId17"/>
+    <tablePart r:id="rId18"/>
   </tableParts>
 </worksheet>
 </file>
@@ -2751,45 +2864,45 @@
   <sheetData>
     <row r="1" customFormat="false" ht="36.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B1" s="23" t="s">
-        <v>148</v>
+        <v>156</v>
       </c>
       <c r="C1" s="23"/>
       <c r="D1" s="23"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="24" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="C3" s="24" t="s">
-        <v>150</v>
+        <v>158</v>
       </c>
       <c r="D3" s="25" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="D4" s="26"/>
     </row>
     <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2886,7 +2999,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="32" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="2" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="C1" s="19"/>
       <c r="D1" s="19"/>
@@ -2897,13 +3010,13 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C2" s="27" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="D2" s="28" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
       <c r="E2" s="28" t="s">
-        <v>158</v>
+        <v>166</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2959,7 +3072,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="32" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="2" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
       <c r="C1" s="19"/>
       <c r="D1" s="19"/>
@@ -2972,31 +3085,31 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="11" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>160</v>
+        <v>168</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>161</v>
+        <v>169</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>162</v>
+        <v>170</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
       <c r="G3" s="33" t="s">
-        <v>164</v>
+        <v>172</v>
       </c>
       <c r="H3" s="34" t="s">
-        <v>165</v>
+        <v>173</v>
       </c>
       <c r="I3" s="34" t="s">
-        <v>166</v>
+        <v>174</v>
       </c>
       <c r="J3" s="34" t="s">
-        <v>167</v>
+        <v>175</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3197,7 +3310,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="32" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="2" t="s">
-        <v>168</v>
+        <v>176</v>
       </c>
       <c r="C1" s="19"/>
       <c r="D1" s="19"/>
@@ -3209,28 +3322,28 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="11" t="s">
-        <v>160</v>
+        <v>168</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>161</v>
+        <v>169</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>162</v>
+        <v>170</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
       <c r="F3" s="33" t="s">
-        <v>164</v>
+        <v>172</v>
       </c>
       <c r="G3" s="34" t="s">
-        <v>165</v>
+        <v>173</v>
       </c>
       <c r="H3" s="34" t="s">
-        <v>166</v>
+        <v>174</v>
       </c>
       <c r="I3" s="48" t="s">
-        <v>167</v>
+        <v>175</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -3292,7 +3405,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="32" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="2" t="s">
-        <v>169</v>
+        <v>177</v>
       </c>
       <c r="C1" s="19"/>
     </row>
@@ -3301,10 +3414,10 @@
     </row>
     <row r="3" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="11" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>170</v>
+        <v>178</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>